<commit_message>
PO average word ssave
</commit_message>
<xml_diff>
--- a/TemplateFiles/EkTemplate.xlsx
+++ b/TemplateFiles/EkTemplate.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="63">
   <si>
     <t>YARIYIL</t>
   </si>
@@ -298,7 +298,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.24995000660419464"/>
+        <fgColor theme="2" tint="-0.24991999566555023"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,7 +334,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.049959998577833176"/>
+        <fgColor theme="0" tint="-0.04992999881505966"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1342,7 +1342,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
       <border/>
@@ -1377,7 +1377,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1414,7 +1414,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
       <border/>
@@ -1422,21 +1422,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1467,7 +1467,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1502,7 +1502,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1512,7 +1512,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1522,7 +1522,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1532,7 +1532,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1542,7 +1542,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1552,7 +1552,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1562,14 +1562,14 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1579,7 +1579,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1589,7 +1589,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1620,7 +1620,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1648,7 +1648,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24991999566555023"/>
+          <bgColor theme="2" tint="-0.24988999962806702"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1878,11 +1878,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="9490050"/>
-        <c:axId val="24399080"/>
+        <c:axId val="43078121"/>
+        <c:axId val="59467286"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="9490050"/>
+        <c:axId val="43078121"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1892,14 +1892,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="24399080"/>
+        <c:crossAx val="59467286"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="24399080"/>
+        <c:axId val="59467286"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1948,7 +1948,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="9490050"/>
+        <c:crossAx val="43078121"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2142,11 +2142,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="24216811"/>
-        <c:axId val="16014678"/>
+        <c:axId val="58782208"/>
+        <c:axId val="27953685"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="24216811"/>
+        <c:axId val="58782208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2156,14 +2156,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="16014678"/>
+        <c:crossAx val="27953685"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="16014678"/>
+        <c:axId val="27953685"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2210,7 +2210,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="24216811"/>
+        <c:crossAx val="58782208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2268,10 +2268,10 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>65</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2280,7 +2280,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="31899225" y="4048125"/>
-        <a:ext cx="10287000" cy="10287000"/>
+        <a:ext cx="4286250" cy="4286250"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3620,180 +3620,426 @@
       <c r="BE5" s="26"/>
     </row>
     <row r="6" spans="1:57" ht="15.75" customHeight="1">
-      <c r="A6" s="148"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="148" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C6" s="141"/>
       <c r="D6" s="39"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
+      <c r="E6" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F6" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G6" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H6" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I6" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J6" s="37">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K6" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="L6" s="37">
+        <v>0.9248000383377075</v>
+      </c>
       <c r="M6" s="38"/>
       <c r="N6" s="39"/>
       <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
+      <c r="P6" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q6" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R6" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S6" s="39">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T6" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U6" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V6" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="W6" s="37">
+        <v>0.6489999890327454</v>
+      </c>
       <c r="X6" s="38"/>
       <c r="Y6" s="39"/>
       <c r="Z6" s="37"/>
-      <c r="AA6" s="37"/>
-      <c r="AB6" s="37"/>
-      <c r="AC6" s="37"/>
-      <c r="AD6" s="37"/>
-      <c r="AE6" s="37"/>
-      <c r="AF6" s="37"/>
-      <c r="AG6" s="37"/>
-      <c r="AH6" s="37"/>
+      <c r="AA6" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB6" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC6" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD6" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE6" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF6" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG6" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AH6" s="37">
+        <v>0.6800000071525574</v>
+      </c>
       <c r="AI6" s="38"/>
       <c r="AJ6" s="36"/>
       <c r="AK6" s="37"/>
-      <c r="AL6" s="37"/>
-      <c r="AM6" s="37"/>
-      <c r="AN6" s="37"/>
-      <c r="AO6" s="37"/>
-      <c r="AP6" s="37"/>
+      <c r="AL6" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM6" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN6" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO6" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP6" s="37">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AQ6" s="37"/>
-      <c r="AR6" s="37"/>
-      <c r="AS6" s="37"/>
+      <c r="AR6" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AS6" s="37">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AT6" s="40"/>
       <c r="AU6" s="26"/>
       <c r="AV6" s="26"/>
-      <c r="AW6" s="26"/>
-      <c r="AX6" s="26"/>
-      <c r="AY6" s="26"/>
-      <c r="AZ6" s="26"/>
-      <c r="BA6" s="26"/>
-      <c r="BB6" s="26"/>
-      <c r="BC6" s="26"/>
-      <c r="BD6" s="26"/>
+      <c r="AW6" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AX6" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY6" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ6" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA6" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB6" s="26">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC6" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BD6" s="26">
+        <v>0.7344500422477722</v>
+      </c>
       <c r="BE6" s="26"/>
     </row>
     <row r="7" spans="1:57" ht="15.75" customHeight="1">
-      <c r="A7" s="79"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C7" s="141"/>
       <c r="D7" s="39"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
+      <c r="E7" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F7" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G7" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H7" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I7" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J7" s="37">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K7" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="L7" s="37">
+        <v>0.9248000383377075</v>
+      </c>
       <c r="M7" s="38"/>
       <c r="N7" s="39"/>
       <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="39"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="37"/>
+      <c r="P7" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q7" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R7" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S7" s="39">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T7" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U7" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V7" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="W7" s="37">
+        <v>0.6489999890327454</v>
+      </c>
       <c r="X7" s="38"/>
       <c r="Y7" s="39"/>
       <c r="Z7" s="37"/>
-      <c r="AA7" s="37"/>
-      <c r="AB7" s="37"/>
-      <c r="AC7" s="37"/>
-      <c r="AD7" s="37"/>
-      <c r="AE7" s="37"/>
-      <c r="AF7" s="37"/>
-      <c r="AG7" s="37"/>
-      <c r="AH7" s="37"/>
+      <c r="AA7" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB7" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC7" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD7" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE7" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF7" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG7" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AH7" s="37">
+        <v>0.6800000071525574</v>
+      </c>
       <c r="AI7" s="38"/>
       <c r="AJ7" s="36"/>
       <c r="AK7" s="37"/>
-      <c r="AL7" s="37"/>
-      <c r="AM7" s="37"/>
-      <c r="AN7" s="37"/>
-      <c r="AO7" s="37"/>
-      <c r="AP7" s="37"/>
+      <c r="AL7" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM7" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN7" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO7" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP7" s="37">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AQ7" s="37"/>
-      <c r="AR7" s="37"/>
-      <c r="AS7" s="37"/>
+      <c r="AR7" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AS7" s="37">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AT7" s="40"/>
       <c r="AU7" s="26"/>
       <c r="AV7" s="26"/>
-      <c r="AW7" s="26"/>
-      <c r="AX7" s="26"/>
-      <c r="AY7" s="26"/>
-      <c r="AZ7" s="26"/>
-      <c r="BA7" s="26"/>
-      <c r="BB7" s="26"/>
-      <c r="BC7" s="26"/>
-      <c r="BD7" s="26"/>
+      <c r="AW7" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AX7" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY7" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ7" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA7" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB7" s="26">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC7" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BD7" s="26">
+        <v>0.7344500422477722</v>
+      </c>
       <c r="BE7" s="26"/>
     </row>
     <row r="8" spans="1:57" ht="15.75" customHeight="1">
-      <c r="A8" s="148"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="148" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C8" s="141"/>
       <c r="D8" s="39"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
+      <c r="E8" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F8" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G8" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H8" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I8" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J8" s="37">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K8" s="37">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="L8" s="37">
+        <v>0.9248000383377075</v>
+      </c>
       <c r="M8" s="38"/>
       <c r="N8" s="39"/>
       <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="63"/>
-      <c r="T8" s="41"/>
-      <c r="U8" s="37"/>
-      <c r="V8" s="37"/>
-      <c r="W8" s="41"/>
+      <c r="P8" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q8" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R8" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S8" s="63">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T8" s="41">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U8" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V8" s="37">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="W8" s="41">
+        <v>0.6489999890327454</v>
+      </c>
       <c r="X8" s="42"/>
       <c r="Y8" s="39"/>
       <c r="Z8" s="37"/>
-      <c r="AA8" s="37"/>
-      <c r="AB8" s="37"/>
-      <c r="AC8" s="37"/>
-      <c r="AD8" s="37"/>
-      <c r="AE8" s="37"/>
-      <c r="AF8" s="37"/>
-      <c r="AG8" s="37"/>
-      <c r="AH8" s="37"/>
+      <c r="AA8" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB8" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC8" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD8" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE8" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF8" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG8" s="37">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AH8" s="37">
+        <v>0.6800000071525574</v>
+      </c>
       <c r="AI8" s="38"/>
       <c r="AJ8" s="36"/>
       <c r="AK8" s="37"/>
-      <c r="AL8" s="37"/>
-      <c r="AM8" s="37"/>
-      <c r="AN8" s="37"/>
-      <c r="AO8" s="37"/>
-      <c r="AP8" s="37"/>
+      <c r="AL8" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM8" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN8" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO8" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP8" s="37">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AQ8" s="37"/>
-      <c r="AR8" s="37"/>
-      <c r="AS8" s="37"/>
+      <c r="AR8" s="37">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AS8" s="37">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AT8" s="40"/>
       <c r="AU8" s="26"/>
       <c r="AV8" s="26"/>
-      <c r="AW8" s="26"/>
-      <c r="AX8" s="26"/>
-      <c r="AY8" s="26"/>
-      <c r="AZ8" s="26"/>
-      <c r="BA8" s="26"/>
-      <c r="BB8" s="26"/>
-      <c r="BC8" s="26"/>
-      <c r="BD8" s="26"/>
+      <c r="AW8" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AX8" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY8" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ8" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA8" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB8" s="26">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC8" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BD8" s="26">
+        <v>0.7344500422477722</v>
+      </c>
       <c r="BE8" s="26"/>
     </row>
     <row r="9" spans="1:57" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
CreateToken Client Requirement added
Users cannot create token through api without client token
</commit_message>
<xml_diff>
--- a/TemplateFiles/EkTemplate.xlsx
+++ b/TemplateFiles/EkTemplate.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="63">
   <si>
     <t>YARIYIL</t>
   </si>
@@ -298,7 +298,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.24987000226974487"/>
+        <fgColor theme="2" tint="-0.2498600035905838"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,7 +334,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.049880001693964005"/>
+        <fgColor theme="0" tint="-0.049869999289512634"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1342,7 +1342,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
       <border/>
@@ -1377,7 +1377,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1414,7 +1414,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
       <border/>
@@ -1422,21 +1422,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1467,7 +1467,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1502,7 +1502,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1512,7 +1512,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1522,7 +1522,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1532,7 +1532,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1542,7 +1542,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1552,7 +1552,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1562,14 +1562,14 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1579,7 +1579,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1589,7 +1589,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1620,7 +1620,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1648,7 +1648,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24984000623226166"/>
+          <bgColor theme="2" tint="-0.2498299926519394"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1878,11 +1878,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="2719861"/>
-        <c:axId val="51620497"/>
+        <c:axId val="18291709"/>
+        <c:axId val="35523344"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2719861"/>
+        <c:axId val="18291709"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1892,14 +1892,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51620497"/>
+        <c:crossAx val="35523344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51620497"/>
+        <c:axId val="35523344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1948,7 +1948,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2719861"/>
+        <c:crossAx val="18291709"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2142,11 +2142,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="35976877"/>
-        <c:axId val="57515226"/>
+        <c:axId val="31087966"/>
+        <c:axId val="52876844"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="35976877"/>
+        <c:axId val="31087966"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2156,14 +2156,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57515226"/>
+        <c:crossAx val="52876844"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57515226"/>
+        <c:axId val="52876844"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2210,7 +2210,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="35976877"/>
+        <c:crossAx val="31087966"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2268,9 +2268,9 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2280,7 +2280,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="31899225" y="4048125"/>
-        <a:ext cx="4572000" cy="4572000"/>
+        <a:ext cx="10287000" cy="10287000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4752,62 +4752,146 @@
       <c r="BE13" s="26"/>
     </row>
     <row r="14" spans="1:57" ht="15.75" customHeight="1">
-      <c r="A14" s="16"/>
-      <c r="B14" s="3"/>
+      <c r="A14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="C14" s="142"/>
       <c r="D14" s="47"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
+      <c r="E14" s="45">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F14" s="45">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G14" s="45">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H14" s="45">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I14" s="45">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J14" s="45">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K14" s="45">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="L14" s="45">
+        <v>0.9248000383377075</v>
+      </c>
       <c r="M14" s="46"/>
       <c r="N14" s="44"/>
       <c r="O14" s="45"/>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="45"/>
-      <c r="S14" s="47"/>
-      <c r="T14" s="45"/>
-      <c r="U14" s="45"/>
-      <c r="V14" s="45"/>
-      <c r="W14" s="45"/>
+      <c r="P14" s="45">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q14" s="45">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R14" s="45">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S14" s="47">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T14" s="45">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U14" s="45">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V14" s="45">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="W14" s="45">
+        <v>0.6489999890327454</v>
+      </c>
       <c r="X14" s="46"/>
       <c r="Y14" s="44"/>
       <c r="Z14" s="45"/>
-      <c r="AA14" s="45"/>
-      <c r="AB14" s="45"/>
-      <c r="AC14" s="45"/>
-      <c r="AD14" s="45"/>
-      <c r="AE14" s="45"/>
-      <c r="AF14" s="45"/>
-      <c r="AG14" s="45"/>
-      <c r="AH14" s="45"/>
+      <c r="AA14" s="45">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB14" s="45">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC14" s="45">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD14" s="45">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE14" s="45">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF14" s="45">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG14" s="45">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AH14" s="45">
+        <v>0.6800000071525574</v>
+      </c>
       <c r="AI14" s="46"/>
-      <c r="AJ14" s="44"/>
+      <c r="AJ14" s="44">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AK14" s="45"/>
       <c r="AL14" s="45"/>
-      <c r="AM14" s="45"/>
-      <c r="AN14" s="45"/>
-      <c r="AO14" s="45"/>
-      <c r="AP14" s="45"/>
+      <c r="AM14" s="45">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN14" s="45">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO14" s="45">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP14" s="45">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AQ14" s="45"/>
-      <c r="AR14" s="45"/>
-      <c r="AS14" s="45"/>
+      <c r="AR14" s="45">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AS14" s="45">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AT14" s="48"/>
-      <c r="AU14" s="26"/>
+      <c r="AU14" s="26">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AV14" s="26"/>
-      <c r="AW14" s="26"/>
-      <c r="AX14" s="26"/>
-      <c r="AY14" s="26"/>
-      <c r="AZ14" s="26"/>
-      <c r="BA14" s="26"/>
-      <c r="BB14" s="26"/>
-      <c r="BC14" s="26"/>
-      <c r="BD14" s="26"/>
+      <c r="AW14" s="26">
+        <v>0.7512667179107666</v>
+      </c>
+      <c r="AX14" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY14" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ14" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA14" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB14" s="26">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC14" s="26">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BD14" s="26">
+        <v>0.7344500422477722</v>
+      </c>
       <c r="BE14" s="26"/>
     </row>
     <row r="15" spans="1:57" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
File Upload Bugfix. Token ExpdateUpdated
</commit_message>
<xml_diff>
--- a/TemplateFiles/EkTemplate.xlsx
+++ b/TemplateFiles/EkTemplate.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="62">
   <si>
     <t>YARIYIL</t>
   </si>
@@ -295,7 +295,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.2496899962425232"/>
+        <fgColor theme="2" tint="-0.24973000586032867"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +331,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.04969999939203262"/>
+        <fgColor theme="0" tint="-0.04974000155925751"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1339,7 +1339,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
       <border/>
@@ -1374,7 +1374,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1411,7 +1411,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
       <border/>
@@ -1419,21 +1419,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1464,7 +1464,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1499,7 +1499,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1509,7 +1509,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1519,7 +1519,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1529,7 +1529,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1539,7 +1539,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1549,7 +1549,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1559,14 +1559,14 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1576,7 +1576,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1586,7 +1586,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1617,7 +1617,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1645,7 +1645,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24966000020503998"/>
+          <bgColor theme="2" tint="-0.24969999492168427"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1875,11 +1875,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="18674121"/>
-        <c:axId val="22213338"/>
+        <c:axId val="25094539"/>
+        <c:axId val="52090828"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="18674121"/>
+        <c:axId val="25094539"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,14 +1889,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="22213338"/>
+        <c:crossAx val="52090828"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22213338"/>
+        <c:axId val="52090828"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1945,7 +1945,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18674121"/>
+        <c:crossAx val="25094539"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2139,11 +2139,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="5334829"/>
-        <c:axId val="44625556"/>
+        <c:axId val="12608798"/>
+        <c:axId val="31767611"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="5334829"/>
+        <c:axId val="12608798"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2153,14 +2153,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44625556"/>
+        <c:crossAx val="31767611"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44625556"/>
+        <c:axId val="31767611"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2207,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5334829"/>
+        <c:crossAx val="12608798"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2265,10 +2265,10 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>65</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2277,7 +2277,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="31899225" y="4048125"/>
-        <a:ext cx="10287000" cy="10287000"/>
+        <a:ext cx="4286250" cy="5238750"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2931,7 +2931,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP31"/>
+  <dimension ref="A1:BP28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -3281,11 +3281,11 @@
         <v>0.6800000071525574</v>
       </c>
       <c r="AI3" s="33"/>
-      <c r="AJ3" s="34"/>
+      <c r="AJ3" s="34">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AK3" s="34"/>
-      <c r="AL3" s="34">
-        <v>0.6840000152587891</v>
-      </c>
+      <c r="AL3" s="34"/>
       <c r="AM3" s="34">
         <v>0.6840000152587891</v>
       </c>
@@ -3306,10 +3306,12 @@
         <v>0.6840000152587891</v>
       </c>
       <c r="AT3" s="32"/>
-      <c r="AU3" s="26"/>
+      <c r="AU3" s="26">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AV3" s="26"/>
       <c r="AW3" s="26">
-        <v>0.7344500422477722</v>
+        <v>0.7512667179107666</v>
       </c>
       <c r="AX3" s="26">
         <v>0.7344500422477722</v>
@@ -3422,11 +3424,11 @@
         <v>0.6800000071525574</v>
       </c>
       <c r="AI4" s="38"/>
-      <c r="AJ4" s="36"/>
+      <c r="AJ4" s="36">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AK4" s="37"/>
-      <c r="AL4" s="37">
-        <v>0.6840000152587891</v>
-      </c>
+      <c r="AL4" s="37"/>
       <c r="AM4" s="37">
         <v>0.6840000152587891</v>
       </c>
@@ -3447,10 +3449,12 @@
         <v>0.6840000152587891</v>
       </c>
       <c r="AT4" s="40"/>
-      <c r="AU4" s="26"/>
+      <c r="AU4" s="26">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AV4" s="26"/>
       <c r="AW4" s="26">
-        <v>0.7344500422477722</v>
+        <v>0.7512667179107666</v>
       </c>
       <c r="AX4" s="26">
         <v>0.7344500422477722</v>
@@ -3563,11 +3567,11 @@
         <v>0.6800000071525574</v>
       </c>
       <c r="AI5" s="38"/>
-      <c r="AJ5" s="36"/>
+      <c r="AJ5" s="36">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AK5" s="37"/>
-      <c r="AL5" s="37">
-        <v>0.6840000152587891</v>
-      </c>
+      <c r="AL5" s="37"/>
       <c r="AM5" s="37">
         <v>0.6840000152587891</v>
       </c>
@@ -3588,10 +3592,12 @@
         <v>0.6840000152587891</v>
       </c>
       <c r="AT5" s="40"/>
-      <c r="AU5" s="26"/>
+      <c r="AU5" s="26">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AV5" s="26"/>
       <c r="AW5" s="26">
-        <v>0.7344500422477722</v>
+        <v>0.7512667179107666</v>
       </c>
       <c r="AX5" s="26">
         <v>0.7344500422477722</v>
@@ -3704,11 +3710,11 @@
         <v>0.6800000071525574</v>
       </c>
       <c r="AI6" s="38"/>
-      <c r="AJ6" s="36"/>
+      <c r="AJ6" s="36">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AK6" s="37"/>
-      <c r="AL6" s="37">
-        <v>0.6840000152587891</v>
-      </c>
+      <c r="AL6" s="37"/>
       <c r="AM6" s="37">
         <v>0.6840000152587891</v>
       </c>
@@ -3729,10 +3735,12 @@
         <v>0.6840000152587891</v>
       </c>
       <c r="AT6" s="40"/>
-      <c r="AU6" s="26"/>
+      <c r="AU6" s="26">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AV6" s="26"/>
       <c r="AW6" s="26">
-        <v>0.7344500422477722</v>
+        <v>0.7512667179107666</v>
       </c>
       <c r="AX6" s="26">
         <v>0.7344500422477722</v>
@@ -3845,11 +3853,11 @@
         <v>0.6800000071525574</v>
       </c>
       <c r="AI7" s="38"/>
-      <c r="AJ7" s="36"/>
+      <c r="AJ7" s="36">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AK7" s="37"/>
-      <c r="AL7" s="37">
-        <v>0.6840000152587891</v>
-      </c>
+      <c r="AL7" s="37"/>
       <c r="AM7" s="37">
         <v>0.6840000152587891</v>
       </c>
@@ -3870,10 +3878,12 @@
         <v>0.6840000152587891</v>
       </c>
       <c r="AT7" s="40"/>
-      <c r="AU7" s="26"/>
+      <c r="AU7" s="26">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AV7" s="26"/>
       <c r="AW7" s="26">
-        <v>0.7344500422477722</v>
+        <v>0.7512667179107666</v>
       </c>
       <c r="AX7" s="26">
         <v>0.7344500422477722</v>
@@ -3986,11 +3996,11 @@
         <v>0.6800000071525574</v>
       </c>
       <c r="AI8" s="38"/>
-      <c r="AJ8" s="36"/>
+      <c r="AJ8" s="36">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AK8" s="37"/>
-      <c r="AL8" s="37">
-        <v>0.6840000152587891</v>
-      </c>
+      <c r="AL8" s="37"/>
       <c r="AM8" s="37">
         <v>0.6840000152587891</v>
       </c>
@@ -4011,10 +4021,12 @@
         <v>0.6840000152587891</v>
       </c>
       <c r="AT8" s="40"/>
-      <c r="AU8" s="26"/>
+      <c r="AU8" s="26">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AV8" s="26"/>
       <c r="AW8" s="26">
-        <v>0.7344500422477722</v>
+        <v>0.7512667179107666</v>
       </c>
       <c r="AX8" s="26">
         <v>0.7344500422477722</v>
@@ -4127,11 +4139,11 @@
         <v>0.6800000071525574</v>
       </c>
       <c r="AI9" s="46"/>
-      <c r="AJ9" s="44"/>
+      <c r="AJ9" s="44">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AK9" s="45"/>
-      <c r="AL9" s="45">
-        <v>0.6840000152587891</v>
-      </c>
+      <c r="AL9" s="45"/>
       <c r="AM9" s="45">
         <v>0.6840000152587891</v>
       </c>
@@ -4152,10 +4164,12 @@
         <v>0.6840000152587891</v>
       </c>
       <c r="AT9" s="48"/>
-      <c r="AU9" s="26"/>
+      <c r="AU9" s="26">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AV9" s="26"/>
       <c r="AW9" s="26">
-        <v>0.7344500422477722</v>
+        <v>0.7512667179107666</v>
       </c>
       <c r="AX9" s="26">
         <v>0.7344500422477722</v>
@@ -4268,11 +4282,11 @@
         <v>0.6800000071525574</v>
       </c>
       <c r="AI10" s="50"/>
-      <c r="AJ10" s="51"/>
+      <c r="AJ10" s="51">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AK10" s="51"/>
-      <c r="AL10" s="51">
-        <v>0.6840000152587891</v>
-      </c>
+      <c r="AL10" s="51"/>
       <c r="AM10" s="51">
         <v>0.6840000152587891</v>
       </c>
@@ -4293,10 +4307,12 @@
         <v>0.6840000152587891</v>
       </c>
       <c r="AT10" s="52"/>
-      <c r="AU10" s="26"/>
+      <c r="AU10" s="26">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AV10" s="26"/>
       <c r="AW10" s="26">
-        <v>0.7344500422477722</v>
+        <v>0.7512667179107666</v>
       </c>
       <c r="AX10" s="26">
         <v>0.7344500422477722</v>
@@ -4409,11 +4425,11 @@
         <v>0.6800000071525574</v>
       </c>
       <c r="AI11" s="38"/>
-      <c r="AJ11" s="36"/>
+      <c r="AJ11" s="36">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AK11" s="37"/>
-      <c r="AL11" s="37">
-        <v>0.6840000152587891</v>
-      </c>
+      <c r="AL11" s="37"/>
       <c r="AM11" s="37">
         <v>0.6840000152587891</v>
       </c>
@@ -4434,10 +4450,12 @@
         <v>0.6840000152587891</v>
       </c>
       <c r="AT11" s="40"/>
-      <c r="AU11" s="26"/>
+      <c r="AU11" s="26">
+        <v>0.6840000152587891</v>
+      </c>
       <c r="AV11" s="26"/>
       <c r="AW11" s="26">
-        <v>0.7344500422477722</v>
+        <v>0.7512667179107666</v>
       </c>
       <c r="AX11" s="26">
         <v>0.7344500422477722</v>
@@ -6648,519 +6666,9 @@
         <v>0.7344500422477722</v>
       </c>
     </row>
-    <row r="28" spans="1:65" ht="15">
-      <c r="A28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="F28">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="G28">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="H28">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="I28">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="J28">
-        <v>0.9371429085731506</v>
-      </c>
-      <c r="K28">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="L28">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="P28">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="Q28">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="R28">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="S28">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="T28">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="U28">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="V28">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="W28">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="AA28">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AB28">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AC28">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AD28">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AE28">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AF28">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AG28">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AH28">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AJ28">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AM28">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AN28">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AO28">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AP28">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AR28">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AS28">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AU28">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AW28">
-        <v>0.7512667179107666</v>
-      </c>
-      <c r="AX28">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="AY28">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="AZ28">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="BA28">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="BB28">
-        <v>0.7553809285163879</v>
-      </c>
-      <c r="BC28">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="BD28">
-        <v>0.7344500422477722</v>
-      </c>
+    <row r="28" ht="15">
       <c r="BM28" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:56" ht="15">
-      <c r="A29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="F29">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="G29">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="H29">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="I29">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="J29">
-        <v>0.9371429085731506</v>
-      </c>
-      <c r="K29">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="L29">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="P29">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="Q29">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="R29">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="S29">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="T29">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="U29">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="V29">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="W29">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="AA29">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AB29">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AC29">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AD29">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AE29">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AF29">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AG29">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AH29">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AJ29">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AM29">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AN29">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AO29">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AP29">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AR29">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AS29">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AU29">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AW29">
-        <v>0.7512667179107666</v>
-      </c>
-      <c r="AX29">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="AY29">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="AZ29">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="BA29">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="BB29">
-        <v>0.7553809285163879</v>
-      </c>
-      <c r="BC29">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="BD29">
-        <v>0.7344500422477722</v>
-      </c>
-    </row>
-    <row r="30" spans="1:56" ht="15">
-      <c r="A30" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="F30">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="G30">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="H30">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="I30">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="J30">
-        <v>0.9371429085731506</v>
-      </c>
-      <c r="K30">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="L30">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="P30">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="Q30">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="R30">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="S30">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="T30">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="U30">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="V30">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="W30">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="AA30">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AB30">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AC30">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AD30">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AE30">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AF30">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AG30">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AH30">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AJ30">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AM30">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AN30">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AO30">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AP30">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AR30">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AS30">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AU30">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AW30">
-        <v>0.7512667179107666</v>
-      </c>
-      <c r="AX30">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="AY30">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="AZ30">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="BA30">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="BB30">
-        <v>0.7553809285163879</v>
-      </c>
-      <c r="BC30">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="BD30">
-        <v>0.7344500422477722</v>
-      </c>
-    </row>
-    <row r="31" spans="1:56" ht="15">
-      <c r="A31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="F31">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="G31">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="H31">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="I31">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="J31">
-        <v>0.9371429085731506</v>
-      </c>
-      <c r="K31">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="L31">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="P31">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="Q31">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="R31">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="S31">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="T31">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="U31">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="V31">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="W31">
-        <v>0.6489999890327454</v>
-      </c>
-      <c r="AA31">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AB31">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AC31">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AD31">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AE31">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AF31">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AG31">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AH31">
-        <v>0.6800000071525574</v>
-      </c>
-      <c r="AJ31">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AM31">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AN31">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AO31">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AP31">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AR31">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AS31">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AU31">
-        <v>0.6840000152587891</v>
-      </c>
-      <c r="AW31">
-        <v>0.7512667179107666</v>
-      </c>
-      <c r="AX31">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="AY31">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="AZ31">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="BA31">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="BB31">
-        <v>0.7553809285163879</v>
-      </c>
-      <c r="BC31">
-        <v>0.7344500422477722</v>
-      </c>
-      <c r="BD31">
-        <v>0.7344500422477722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
result file divided by worksheetname
</commit_message>
<xml_diff>
--- a/TemplateFiles/EkTemplate.xlsx
+++ b/TemplateFiles/EkTemplate.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="62">
   <si>
     <t>YARIYIL</t>
   </si>
@@ -295,7 +295,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.24973000586032867"/>
+        <fgColor theme="2" tint="-0.2497200071811676"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +331,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.04974000155925751"/>
+        <fgColor theme="0" tint="-0.04972999915480614"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1339,7 +1339,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
       <border/>
@@ -1374,7 +1374,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1411,7 +1411,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
       <border/>
@@ -1419,21 +1419,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1464,7 +1464,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1499,7 +1499,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1509,7 +1509,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1519,7 +1519,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1529,7 +1529,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1539,7 +1539,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1549,7 +1549,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1559,14 +1559,14 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1576,7 +1576,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1586,7 +1586,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1617,7 +1617,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1645,7 +1645,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24969999492168427"/>
+          <bgColor theme="2" tint="-0.2496899962425232"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1875,11 +1875,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="25094539"/>
-        <c:axId val="52090828"/>
+        <c:axId val="53960571"/>
+        <c:axId val="12306622"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="25094539"/>
+        <c:axId val="53960571"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,14 +1889,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52090828"/>
+        <c:crossAx val="12306622"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52090828"/>
+        <c:axId val="12306622"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1945,7 +1945,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="25094539"/>
+        <c:crossAx val="53960571"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2139,11 +2139,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="12608798"/>
-        <c:axId val="31767611"/>
+        <c:axId val="16927107"/>
+        <c:axId val="23522335"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="12608798"/>
+        <c:axId val="16927107"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2153,14 +2153,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="31767611"/>
+        <c:crossAx val="23522335"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31767611"/>
+        <c:axId val="23522335"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2207,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="12608798"/>
+        <c:crossAx val="16927107"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -6666,7 +6666,133 @@
         <v>0.7344500422477722</v>
       </c>
     </row>
-    <row r="28" ht="15">
+    <row r="28" spans="1:65" ht="15">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F28">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G28">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H28">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I28">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J28">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K28">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="L28">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="P28">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q28">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R28">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S28">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T28">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U28">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V28">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="W28">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="AA28">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB28">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC28">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD28">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE28">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF28">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG28">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AH28">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AJ28">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM28">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN28">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO28">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP28">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AR28">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AS28">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AU28">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AW28">
+        <v>0.7512667179107666</v>
+      </c>
+      <c r="AX28">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY28">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ28">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA28">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB28">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC28">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BD28">
+        <v>0.7344500422477722</v>
+      </c>
       <c r="BM28" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Result downloand file as zip file
</commit_message>
<xml_diff>
--- a/TemplateFiles/EkTemplate.xlsx
+++ b/TemplateFiles/EkTemplate.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="62">
   <si>
     <t>YARIYIL</t>
   </si>
@@ -295,7 +295,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.2497200071811676"/>
+        <fgColor theme="2" tint="-0.24967999756336212"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +331,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.04972999915480614"/>
+        <fgColor theme="0" tint="-0.04969000071287155"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1339,7 +1339,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
       <border/>
@@ -1374,7 +1374,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1411,7 +1411,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
       <border/>
@@ -1419,21 +1419,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1464,7 +1464,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1499,7 +1499,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1509,7 +1509,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1519,7 +1519,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1529,7 +1529,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1539,7 +1539,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1549,7 +1549,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1559,14 +1559,14 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1576,7 +1576,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1586,7 +1586,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1617,7 +1617,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1645,7 +1645,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496899962425232"/>
+          <bgColor theme="2" tint="-0.2496500015258789"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1875,11 +1875,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="53960571"/>
-        <c:axId val="12306622"/>
+        <c:axId val="44292092"/>
+        <c:axId val="41621279"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="53960571"/>
+        <c:axId val="44292092"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,14 +1889,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="12306622"/>
+        <c:crossAx val="41621279"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12306622"/>
+        <c:axId val="41621279"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1945,7 +1945,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53960571"/>
+        <c:crossAx val="44292092"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2139,11 +2139,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="16927107"/>
-        <c:axId val="23522335"/>
+        <c:axId val="23602695"/>
+        <c:axId val="3176390"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="16927107"/>
+        <c:axId val="23602695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2153,14 +2153,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="23522335"/>
+        <c:crossAx val="3176390"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23522335"/>
+        <c:axId val="3176390"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2207,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="16927107"/>
+        <c:crossAx val="23602695"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2931,7 +2931,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP28"/>
+  <dimension ref="A1:BP32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -6795,6 +6795,518 @@
       </c>
       <c r="BM28" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:56" ht="15">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F29">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G29">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H29">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I29">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J29">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K29">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="L29">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="P29">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q29">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R29">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S29">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T29">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U29">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V29">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="W29">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="AA29">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB29">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC29">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD29">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE29">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF29">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG29">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AH29">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AJ29">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM29">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN29">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO29">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP29">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AR29">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AS29">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AU29">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AW29">
+        <v>0.7512667179107666</v>
+      </c>
+      <c r="AX29">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY29">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ29">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA29">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB29">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC29">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BD29">
+        <v>0.7344500422477722</v>
+      </c>
+    </row>
+    <row r="30" spans="1:56" ht="15">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F30">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G30">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H30">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I30">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J30">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K30">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="L30">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="P30">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q30">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R30">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S30">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T30">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U30">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V30">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="W30">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="AA30">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB30">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC30">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD30">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE30">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF30">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG30">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AH30">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AJ30">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM30">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN30">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO30">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP30">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AR30">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AS30">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AU30">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AW30">
+        <v>0.7512667179107666</v>
+      </c>
+      <c r="AX30">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY30">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ30">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA30">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB30">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC30">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BD30">
+        <v>0.7344500422477722</v>
+      </c>
+    </row>
+    <row r="31" spans="1:56" ht="15">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F31">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G31">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H31">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I31">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J31">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K31">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="L31">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="P31">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q31">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R31">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S31">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T31">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U31">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V31">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="W31">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="AA31">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB31">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC31">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD31">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE31">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF31">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG31">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AH31">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AJ31">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM31">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN31">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO31">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP31">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AR31">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AS31">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AU31">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AW31">
+        <v>0.7512667179107666</v>
+      </c>
+      <c r="AX31">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY31">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ31">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA31">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB31">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC31">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BD31">
+        <v>0.7344500422477722</v>
+      </c>
+    </row>
+    <row r="32" spans="1:56" ht="15">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F32">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G32">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H32">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I32">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J32">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K32">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="L32">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="P32">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q32">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R32">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S32">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T32">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U32">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V32">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="W32">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="AA32">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB32">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC32">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD32">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE32">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF32">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG32">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AH32">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AJ32">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM32">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN32">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO32">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP32">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AR32">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AS32">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AU32">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AW32">
+        <v>0.7512667179107666</v>
+      </c>
+      <c r="AX32">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY32">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ32">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA32">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB32">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC32">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BD32">
+        <v>0.7344500422477722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PopUp ui changes. User result ready courses added
</commit_message>
<xml_diff>
--- a/TemplateFiles/EkTemplate.xlsx
+++ b/TemplateFiles/EkTemplate.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="62">
   <si>
     <t>YARIYIL</t>
   </si>
@@ -295,7 +295,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.24967999756336212"/>
+        <fgColor theme="2" tint="-0.2496500015258789"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +331,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.04969000071287155"/>
+        <fgColor theme="0" tint="-0.04966000095009804"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1339,7 +1339,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
       <border/>
@@ -1374,7 +1374,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1411,7 +1411,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
       <border/>
@@ -1419,21 +1419,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1464,7 +1464,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1499,7 +1499,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1509,7 +1509,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1519,7 +1519,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1529,7 +1529,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1539,7 +1539,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1549,7 +1549,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1559,14 +1559,14 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1576,7 +1576,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1586,7 +1586,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1617,7 +1617,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1645,7 +1645,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496500015258789"/>
+          <bgColor theme="2" tint="-0.2496200054883957"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1875,11 +1875,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="44292092"/>
-        <c:axId val="41621279"/>
+        <c:axId val="22322349"/>
+        <c:axId val="64981649"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="44292092"/>
+        <c:axId val="22322349"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,14 +1889,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41621279"/>
+        <c:crossAx val="64981649"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41621279"/>
+        <c:axId val="64981649"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1945,7 +1945,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44292092"/>
+        <c:crossAx val="22322349"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2139,11 +2139,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="23602695"/>
-        <c:axId val="3176390"/>
+        <c:axId val="38493088"/>
+        <c:axId val="54467399"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="23602695"/>
+        <c:axId val="38493088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2153,14 +2153,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3176390"/>
+        <c:crossAx val="54467399"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3176390"/>
+        <c:axId val="54467399"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2207,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="23602695"/>
+        <c:crossAx val="38493088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2931,7 +2931,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP32"/>
+  <dimension ref="A1:BP35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -7306,6 +7306,348 @@
         <v>0.7344500422477722</v>
       </c>
       <c r="BD32">
+        <v>0.7344500422477722</v>
+      </c>
+    </row>
+    <row r="33" spans="1:55" ht="15">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F33">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G33">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H33">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I33">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J33">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K33">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="L33">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="P33">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q33">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R33">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S33">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T33">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U33">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V33">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="AA33">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB33">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC33">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD33">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE33">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF33">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG33">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AJ33">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM33">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN33">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO33">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP33">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AR33">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AU33">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AW33">
+        <v>0.7512667179107666</v>
+      </c>
+      <c r="AX33">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY33">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ33">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA33">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB33">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC33">
+        <v>0.7344500422477722</v>
+      </c>
+    </row>
+    <row r="34" spans="1:55" ht="15">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F34">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G34">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H34">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I34">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J34">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K34">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="P34">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q34">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R34">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S34">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T34">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U34">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V34">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="AA34">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB34">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC34">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD34">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE34">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF34">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG34">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AJ34">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM34">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN34">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO34">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP34">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AR34">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AU34">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AW34">
+        <v>0.7512667179107666</v>
+      </c>
+      <c r="AX34">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY34">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ34">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA34">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB34">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC34">
+        <v>0.7344500422477722</v>
+      </c>
+    </row>
+    <row r="35" spans="1:55" ht="15">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F35">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G35">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H35">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I35">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J35">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K35">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="P35">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q35">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R35">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S35">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T35">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U35">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V35">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="AA35">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB35">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC35">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD35">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE35">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF35">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG35">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AJ35">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM35">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN35">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO35">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP35">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AR35">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AU35">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AW35">
+        <v>0.7512667179107666</v>
+      </c>
+      <c r="AX35">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY35">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ35">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA35">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB35">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC35">
         <v>0.7344500422477722</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Session token expiration situations implemented
when user is in active for 10 minute popup will alert the user and will refresh the user or logout.
when user sends a request but its session token is expired it will update its session and refresh token
</commit_message>
<xml_diff>
--- a/TemplateFiles/EkTemplate.xlsx
+++ b/TemplateFiles/EkTemplate.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="62">
   <si>
     <t>YARIYIL</t>
   </si>
@@ -295,7 +295,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.2496500015258789"/>
+        <fgColor theme="2" tint="-0.24964000284671783"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +331,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.04966000095009804"/>
+        <fgColor theme="0" tint="-0.04964999854564667"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1339,7 +1339,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
       <border/>
@@ -1374,7 +1374,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1411,7 +1411,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
       <border/>
@@ -1419,21 +1419,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1464,7 +1464,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1499,7 +1499,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1509,7 +1509,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1519,7 +1519,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1529,7 +1529,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1539,7 +1539,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1549,7 +1549,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1559,14 +1559,14 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1576,7 +1576,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1586,7 +1586,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1617,7 +1617,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1645,7 +1645,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2496200054883957"/>
+          <bgColor theme="2" tint="-0.24961000680923462"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1875,11 +1875,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="22322349"/>
-        <c:axId val="64981649"/>
+        <c:axId val="27084294"/>
+        <c:axId val="46344233"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="22322349"/>
+        <c:axId val="27084294"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,14 +1889,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64981649"/>
+        <c:crossAx val="46344233"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64981649"/>
+        <c:axId val="46344233"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1945,7 +1945,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="22322349"/>
+        <c:crossAx val="27084294"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2139,11 +2139,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="38493088"/>
-        <c:axId val="54467399"/>
+        <c:axId val="62895360"/>
+        <c:axId val="61359409"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="38493088"/>
+        <c:axId val="62895360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2153,14 +2153,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54467399"/>
+        <c:crossAx val="61359409"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54467399"/>
+        <c:axId val="61359409"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2207,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38493088"/>
+        <c:crossAx val="62895360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2931,7 +2931,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP35"/>
+  <dimension ref="A1:BP36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -7648,6 +7648,119 @@
         <v>0.7553809285163879</v>
       </c>
       <c r="BC35">
+        <v>0.7344500422477722</v>
+      </c>
+    </row>
+    <row r="36" spans="1:55" ht="15">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F36">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G36">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H36">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I36">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J36">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K36">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="P36">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q36">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R36">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S36">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T36">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U36">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V36">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="AA36">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB36">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC36">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD36">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE36">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF36">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG36">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AJ36">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM36">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN36">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO36">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP36">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AR36">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AU36">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AW36">
+        <v>0.7512667179107666</v>
+      </c>
+      <c r="AX36">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY36">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ36">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA36">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB36">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC36">
         <v>0.7344500422477722</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Admin User search Page added
</commit_message>
<xml_diff>
--- a/TemplateFiles/EkTemplate.xlsx
+++ b/TemplateFiles/EkTemplate.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="62">
   <si>
     <t>YARIYIL</t>
   </si>
@@ -295,7 +295,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.24945999681949615"/>
+        <fgColor theme="2" tint="-0.24944999814033508"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +331,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.049469999969005585"/>
+        <fgColor theme="0" tint="-0.04946000128984451"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1339,7 +1339,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
       <border/>
@@ -1374,7 +1374,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1411,7 +1411,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
       <border/>
@@ -1419,21 +1419,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1464,7 +1464,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1499,7 +1499,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1509,7 +1509,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1519,7 +1519,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1529,7 +1529,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1539,7 +1539,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1549,7 +1549,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1559,14 +1559,14 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1576,7 +1576,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1586,7 +1586,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1617,7 +1617,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1645,7 +1645,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24943000078201294"/>
+          <bgColor theme="2" tint="-0.24942000210285187"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1875,11 +1875,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="15253831"/>
-        <c:axId val="15413706"/>
+        <c:axId val="56526037"/>
+        <c:axId val="758648"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="15253831"/>
+        <c:axId val="56526037"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,14 +1889,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="15413706"/>
+        <c:crossAx val="758648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15413706"/>
+        <c:axId val="758648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1945,7 +1945,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="15253831"/>
+        <c:crossAx val="56526037"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2139,11 +2139,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="29642627"/>
-        <c:axId val="20948170"/>
+        <c:axId val="43242969"/>
+        <c:axId val="48930178"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="29642627"/>
+        <c:axId val="43242969"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2153,14 +2153,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="20948170"/>
+        <c:crossAx val="48930178"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20948170"/>
+        <c:axId val="48930178"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2207,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="29642627"/>
+        <c:crossAx val="43242969"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2931,7 +2931,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP54"/>
+  <dimension ref="A1:BP55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -9795,6 +9795,119 @@
         <v>0.7553809285163879</v>
       </c>
       <c r="BC54">
+        <v>0.7344500422477722</v>
+      </c>
+    </row>
+    <row r="55" spans="1:55" ht="15">
+      <c r="A55" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="E55">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F55">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G55">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H55">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I55">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J55">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K55">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="P55">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q55">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R55">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S55">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T55">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U55">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V55">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="AA55">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB55">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC55">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD55">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE55">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF55">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG55">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AJ55">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM55">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN55">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO55">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP55">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AR55">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AU55">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AW55">
+        <v>0.7512667179107666</v>
+      </c>
+      <c r="AX55">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY55">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ55">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA55">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB55">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC55">
         <v>0.7344500422477722</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Middleware requestpath updated. Business api endpoints misscall fixed
</commit_message>
<xml_diff>
--- a/TemplateFiles/EkTemplate.xlsx
+++ b/TemplateFiles/EkTemplate.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="62">
   <si>
     <t>YARIYIL</t>
   </si>
@@ -295,7 +295,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.24944999814033508"/>
+        <fgColor theme="2" tint="-0.249439999461174"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +331,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.04946000128984451"/>
+        <fgColor theme="0" tint="-0.04944999888539314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1339,7 +1339,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
       <border/>
@@ -1374,7 +1374,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1411,7 +1411,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
       <border/>
@@ -1419,21 +1419,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1464,7 +1464,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1499,7 +1499,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1509,7 +1509,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1519,7 +1519,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1529,7 +1529,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1539,7 +1539,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1549,7 +1549,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1559,14 +1559,14 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1576,7 +1576,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1586,7 +1586,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1617,7 +1617,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1645,7 +1645,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24942000210285187"/>
+          <bgColor theme="2" tint="-0.2494100034236908"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1875,11 +1875,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="56526037"/>
-        <c:axId val="758648"/>
+        <c:axId val="648799"/>
+        <c:axId val="11029592"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="56526037"/>
+        <c:axId val="648799"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,14 +1889,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="758648"/>
+        <c:crossAx val="11029592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="758648"/>
+        <c:axId val="11029592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1945,7 +1945,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56526037"/>
+        <c:crossAx val="648799"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2139,11 +2139,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="43242969"/>
-        <c:axId val="48930178"/>
+        <c:axId val="53285350"/>
+        <c:axId val="33435724"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="43242969"/>
+        <c:axId val="53285350"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2153,14 +2153,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48930178"/>
+        <c:crossAx val="33435724"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48930178"/>
+        <c:axId val="33435724"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2207,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43242969"/>
+        <c:crossAx val="53285350"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2931,7 +2931,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP55"/>
+  <dimension ref="A1:BP56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -9908,6 +9908,119 @@
         <v>0.7553809285163879</v>
       </c>
       <c r="BC55">
+        <v>0.7344500422477722</v>
+      </c>
+    </row>
+    <row r="56" spans="1:55" ht="15">
+      <c r="A56" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" t="s">
+        <v>47</v>
+      </c>
+      <c r="E56">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F56">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G56">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H56">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I56">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J56">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K56">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="P56">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q56">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R56">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S56">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T56">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U56">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V56">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="AA56">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB56">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC56">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD56">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE56">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF56">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG56">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AJ56">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM56">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN56">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO56">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP56">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AR56">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AU56">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AW56">
+        <v>0.7512667179107666</v>
+      </c>
+      <c r="AX56">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY56">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ56">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA56">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB56">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC56">
         <v>0.7344500422477722</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MVC AdminCourser services added,   AdminUserServicesUpdated
Admin user services's api endpoints were not accepting pages it is fixed.
Admin course page get completed
</commit_message>
<xml_diff>
--- a/TemplateFiles/EkTemplate.xlsx
+++ b/TemplateFiles/EkTemplate.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="62">
   <si>
     <t>YARIYIL</t>
   </si>
@@ -295,7 +295,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249439999461174"/>
+        <fgColor theme="2" tint="-0.24943000078201294"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +331,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.04944999888539314"/>
+        <fgColor theme="0" tint="-0.04944000020623207"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1339,7 +1339,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
       <border/>
@@ -1374,7 +1374,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1411,7 +1411,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
       <border/>
@@ -1419,21 +1419,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1464,7 +1464,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1499,7 +1499,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1509,7 +1509,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1519,7 +1519,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1529,7 +1529,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1539,7 +1539,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1549,7 +1549,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1559,14 +1559,14 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1576,7 +1576,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1586,7 +1586,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1617,7 +1617,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1645,7 +1645,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.2494100034236908"/>
+          <bgColor theme="2" tint="-0.24940000474452972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1875,11 +1875,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="648799"/>
-        <c:axId val="11029592"/>
+        <c:axId val="26601913"/>
+        <c:axId val="48393575"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="648799"/>
+        <c:axId val="26601913"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,14 +1889,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="11029592"/>
+        <c:crossAx val="48393575"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11029592"/>
+        <c:axId val="48393575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1945,7 +1945,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="648799"/>
+        <c:crossAx val="26601913"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2139,11 +2139,11 @@
           <c:shape val="box"/>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="53285350"/>
-        <c:axId val="33435724"/>
+        <c:axId val="61003505"/>
+        <c:axId val="60402505"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="53285350"/>
+        <c:axId val="61003505"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2153,14 +2153,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="33435724"/>
+        <c:crossAx val="60402505"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="33435724"/>
+        <c:axId val="60402505"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2207,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53285350"/>
+        <c:crossAx val="61003505"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits/>
@@ -2931,7 +2931,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP56"/>
+  <dimension ref="A1:BP57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -10021,6 +10021,119 @@
         <v>0.7553809285163879</v>
       </c>
       <c r="BC56">
+        <v>0.7344500422477722</v>
+      </c>
+    </row>
+    <row r="57" spans="1:55" ht="15">
+      <c r="A57" t="s">
+        <v>46</v>
+      </c>
+      <c r="B57" t="s">
+        <v>47</v>
+      </c>
+      <c r="E57">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="F57">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="G57">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="H57">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="I57">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="J57">
+        <v>0.9371429085731506</v>
+      </c>
+      <c r="K57">
+        <v>0.9248000383377075</v>
+      </c>
+      <c r="P57">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="Q57">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="R57">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="S57">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="T57">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="U57">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="V57">
+        <v>0.6489999890327454</v>
+      </c>
+      <c r="AA57">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AB57">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AC57">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AD57">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AE57">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AF57">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AG57">
+        <v>0.6800000071525574</v>
+      </c>
+      <c r="AJ57">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AM57">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AN57">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AO57">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AP57">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AR57">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AU57">
+        <v>0.6840000152587891</v>
+      </c>
+      <c r="AW57">
+        <v>0.7512667179107666</v>
+      </c>
+      <c r="AX57">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AY57">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="AZ57">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BA57">
+        <v>0.7344500422477722</v>
+      </c>
+      <c r="BB57">
+        <v>0.7553809285163879</v>
+      </c>
+      <c r="BC57">
         <v>0.7344500422477722</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Admin user page active courses bugfix
</commit_message>
<xml_diff>
--- a/TemplateFiles/EkTemplate.xlsx
+++ b/TemplateFiles/EkTemplate.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27618"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27706"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{7107E171-DCAC-478E-B8C8-7CCC7F5205DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99A6B8C1-7465-4833-B0FB-CEA494E93D3E}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{7107E171-DCAC-478E-B8C8-7CCC7F5205DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DFADDFF-7FBE-420A-B9EC-7BBEA65EFDF7}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,7 @@
     <sheet name="PÇ Destekleme Oranları" sheetId="6" r:id="rId3"/>
     <sheet name="EK5-PÇ Karşılama Yüzdeleri (2)" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="61">
   <si>
     <t>YARIYIL</t>
   </si>
@@ -223,7 +223,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -315,7 +314,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.049989318521683403"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1138,579 +1137,579 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" applyNumberFormat="0" fontId="3" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="2" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="23" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="14" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="35" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="3" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="3" applyFill="1" borderId="11" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="6" applyFill="1" borderId="28" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="6" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="6" applyFill="1" borderId="11" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="9" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="14" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="15" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="7" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="9" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="16" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="10" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="30" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="31" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="32" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="17" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="8" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="11" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="15" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="7" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="11" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="27" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="28" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="11" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="3" applyFill="1" borderId="28" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="8" applyFill="1" borderId="20" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="8" applyFill="1" borderId="12" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="8" applyFill="1" borderId="13" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="41" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="28" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="9" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="5" applyFill="1" borderId="36" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="36" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="46" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="25" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="26" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="9" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="27" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="47" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="44" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="9" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="8" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="46" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="54" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="51" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="55" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="25" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" borderId="18" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" borderId="52" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="38" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="39" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="40" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="33" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="16" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="21" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="45" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="22" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="42" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="3" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="8" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="34" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="2" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="12" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="29" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="13" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="28" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="10" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="11" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="35" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="14" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="43" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="17" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="5" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="23" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="9" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="9" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="5" applyFill="1" borderId="27" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="9" applyFill="1" borderId="9" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" applyFont="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="60" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="62" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="5" applyFill="1" borderId="25" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="25" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="5" applyFill="1" borderId="26" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="26" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="27" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="15" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="7" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="9" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="15" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="7" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="9" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="11" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="11" applyFill="1" borderId="9" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="12" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="9" applyFill="1" borderId="15" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="12" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="9" applyFill="1" borderId="16" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="15" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="7" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="9" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="8" applyFill="1" borderId="15" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="8" applyFill="1" borderId="16" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="8" applyFill="1" borderId="17" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="6" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="6" applyFill="1" borderId="6" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="3" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="3" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="3" applyFill="1" borderId="6" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="12" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="21" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="19" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="24" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="6" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="48" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="49" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="50" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="30" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="37" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="53" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="24" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="56" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="57" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="7" applyFill="1" borderId="58" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="10" applyFill="1" borderId="56" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="10" applyFill="1" borderId="57" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="10" applyFill="1" borderId="58" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="6" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="59" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -2993,16 +2992,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="1" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" bestFit="1" width="50" customWidth="1"/>
-    <col min="4" max="4" bestFit="1" width="36.140625" customWidth="1"/>
-    <col min="5" max="5" bestFit="1" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" bestFit="1" width="36.140625" customWidth="1"/>
-    <col min="7" max="7" bestFit="1" width="37.140625" customWidth="1"/>
-    <col min="8" max="8" bestFit="1" width="40.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -3028,7 +3027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8">
       <c r="A2" s="154" t="s">
         <v>8</v>
       </c>
@@ -3046,7 +3045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8">
       <c r="A3" s="155"/>
       <c r="B3" s="17"/>
       <c r="C3" s="24"/>
@@ -3062,7 +3061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8">
       <c r="A4" s="155"/>
       <c r="B4" s="150"/>
       <c r="C4" s="24"/>
@@ -3076,7 +3075,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8">
       <c r="A5" s="155"/>
       <c r="B5" s="150"/>
       <c r="C5" s="24"/>
@@ -3092,7 +3091,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8">
       <c r="A6" s="155"/>
       <c r="B6" s="126"/>
       <c r="C6" s="24"/>
@@ -3106,7 +3105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8">
       <c r="A7" s="155"/>
       <c r="B7" s="150"/>
       <c r="C7" s="24"/>
@@ -3120,7 +3119,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" ht="15.75">
+    <row r="8" spans="1:8" ht="15.75">
       <c r="A8" s="156"/>
       <c r="B8" s="146"/>
       <c r="C8" s="25"/>
@@ -3132,7 +3131,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8">
       <c r="A9" s="154" t="s">
         <v>15</v>
       </c>
@@ -3150,7 +3149,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8">
       <c r="A10" s="155"/>
       <c r="B10" s="17"/>
       <c r="C10" s="24"/>
@@ -3170,7 +3169,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8">
       <c r="A11" s="155"/>
       <c r="B11" s="17"/>
       <c r="C11" s="24"/>
@@ -3188,7 +3187,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8">
       <c r="A12" s="155"/>
       <c r="B12" s="17"/>
       <c r="C12" s="24"/>
@@ -3206,7 +3205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" ht="15.75">
+    <row r="13" spans="1:8" ht="15.75">
       <c r="A13" s="156"/>
       <c r="B13" s="19"/>
       <c r="C13" s="25"/>
@@ -3222,7 +3221,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8">
       <c r="A14" s="154" t="s">
         <v>26</v>
       </c>
@@ -3240,7 +3239,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8">
       <c r="A15" s="155"/>
       <c r="B15" s="17"/>
       <c r="C15" s="24"/>
@@ -3258,7 +3257,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" ht="15.75">
+    <row r="16" spans="1:8" ht="15.75">
       <c r="A16" s="156"/>
       <c r="B16" s="127"/>
       <c r="C16" s="25"/>
@@ -3272,30 +3271,29 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="3:7">
       <c r="C18" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20">
-      <c r="G20" s="0" t="s">
+    <row r="20" spans="3:7">
+      <c r="G20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25">
-      <c r="F25" s="0" t="s">
+    <row r="25" spans="3:7">
+      <c r="F25" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="3">
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A14:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
@@ -3304,24 +3302,24 @@
   <dimension ref="A1:BP28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="50" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" customWidth="1"/>
     <col min="14" max="14" width="7.7109375" customWidth="1"/>
     <col min="18" max="19" width="7.7109375" customWidth="1"/>
     <col min="21" max="21" width="7.7109375" customWidth="1"/>
-    <col min="58" max="58" bestFit="1" width="9.5703125" customWidth="1"/>
+    <col min="58" max="58" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:57">
       <c r="A1" s="166" t="s">
         <v>32</v>
       </c>
@@ -3394,7 +3392,7 @@
       <c r="BD1" s="158"/>
       <c r="BE1" s="159"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:57" ht="15.75" customHeight="1">
       <c r="A2" s="167"/>
       <c r="B2" s="169"/>
       <c r="C2" s="69" t="s">
@@ -3563,32 +3561,18 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:57" ht="15.75" customHeight="1">
       <c r="A3" s="14"/>
       <c r="B3" s="2"/>
       <c r="C3" s="140"/>
       <c r="D3" s="31"/>
-      <c r="E3" s="32">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="F3" s="32">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="G3" s="32">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="H3" s="32">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="I3" s="32">
-        <v>0.9248000383377075</v>
-      </c>
-      <c r="J3" s="32">
-        <v>0.9371429085731506</v>
-      </c>
-      <c r="K3" s="32">
-        <v>0.9248000383377075</v>
-      </c>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="32"/>
       <c r="M3" s="33"/>
       <c r="N3" s="31"/>
@@ -3636,7 +3620,7 @@
       <c r="BD3" s="26"/>
       <c r="BE3" s="26"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:57" ht="15.75" customHeight="1">
       <c r="A4" s="15"/>
       <c r="B4" s="1"/>
       <c r="C4" s="141"/>
@@ -3695,7 +3679,7 @@
       <c r="BD4" s="26"/>
       <c r="BE4" s="26"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:57" ht="15.75" customHeight="1">
       <c r="A5" s="148"/>
       <c r="B5" s="1"/>
       <c r="C5" s="141"/>
@@ -3754,7 +3738,7 @@
       <c r="BD5" s="26"/>
       <c r="BE5" s="26"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:57" ht="15.75" customHeight="1">
       <c r="A6" s="148"/>
       <c r="B6" s="1"/>
       <c r="C6" s="141"/>
@@ -3813,7 +3797,7 @@
       <c r="BD6" s="26"/>
       <c r="BE6" s="26"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:57" ht="15.75" customHeight="1">
       <c r="A7" s="79"/>
       <c r="B7" s="1"/>
       <c r="C7" s="141"/>
@@ -3872,7 +3856,7 @@
       <c r="BD7" s="26"/>
       <c r="BE7" s="26"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:57" ht="15.75" customHeight="1">
       <c r="A8" s="148"/>
       <c r="B8" s="1"/>
       <c r="C8" s="141"/>
@@ -3931,7 +3915,7 @@
       <c r="BD8" s="26"/>
       <c r="BE8" s="26"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:57" ht="15.75" customHeight="1">
       <c r="A9" s="147"/>
       <c r="B9" s="3"/>
       <c r="C9" s="142"/>
@@ -3990,7 +3974,7 @@
       <c r="BD9" s="26"/>
       <c r="BE9" s="26"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:57" ht="15.75" customHeight="1">
       <c r="A10" s="149"/>
       <c r="B10" s="2"/>
       <c r="C10" s="140"/>
@@ -4049,7 +4033,7 @@
       <c r="BD10" s="26"/>
       <c r="BE10" s="26"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:57" ht="15.75" customHeight="1">
       <c r="A11" s="15"/>
       <c r="B11" s="1"/>
       <c r="C11" s="141"/>
@@ -4108,7 +4092,7 @@
       <c r="BD11" s="26"/>
       <c r="BE11" s="26"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:57" ht="15.75" customHeight="1">
       <c r="A12" s="148"/>
       <c r="B12" s="1"/>
       <c r="C12" s="141"/>
@@ -4167,7 +4151,7 @@
       <c r="BD12" s="26"/>
       <c r="BE12" s="26"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:57" ht="15.75" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="1"/>
       <c r="C13" s="141"/>
@@ -4226,7 +4210,7 @@
       <c r="BD13" s="26"/>
       <c r="BE13" s="26"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:57" ht="15.75" customHeight="1">
       <c r="A14" s="16"/>
       <c r="B14" s="3"/>
       <c r="C14" s="142"/>
@@ -4285,7 +4269,7 @@
       <c r="BD14" s="26"/>
       <c r="BE14" s="26"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:57" ht="15.75" customHeight="1">
       <c r="A15" s="149"/>
       <c r="B15" s="2"/>
       <c r="C15" s="140"/>
@@ -4344,7 +4328,7 @@
       <c r="BD15" s="26"/>
       <c r="BE15" s="26"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:57" ht="15.75" customHeight="1">
       <c r="A16" s="15"/>
       <c r="B16" s="1"/>
       <c r="C16" s="141"/>
@@ -4403,7 +4387,7 @@
       <c r="BD16" s="26"/>
       <c r="BE16" s="26"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:68" ht="15.75" customHeight="1">
       <c r="A17" s="129"/>
       <c r="B17" s="3"/>
       <c r="C17" s="142"/>
@@ -4462,7 +4446,7 @@
       <c r="BD17" s="26"/>
       <c r="BE17" s="26"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:68">
       <c r="BB19" s="160" t="s">
         <v>46</v>
       </c>
@@ -4514,18 +4498,18 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22">
-      <c r="BM22" s="0" t="s">
+    <row r="22" spans="1:68">
+      <c r="BM22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28">
-      <c r="BM28" s="0" t="s">
+    <row r="28" spans="1:68">
+      <c r="BM28" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="7">
     <mergeCell ref="AU1:BE1"/>
     <mergeCell ref="BB19:BE19"/>
     <mergeCell ref="Y1:AI1"/>
@@ -4535,48 +4519,47 @@
     <mergeCell ref="C1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C17">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="17" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:T17 W3:X17">
-    <cfRule type="cellIs" dxfId="2" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3:AI7 Y9:AI17 Y8:AD8 AF8:AI8">
-    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3:AT17">
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:M17">
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU3:BE17">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:X17">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE8">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -4592,15 +4575,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="50.85546875" customWidth="1"/>
-    <col min="14" max="14" bestFit="1" width="33.7109375" customWidth="1"/>
-    <col min="15" max="15" bestFit="1" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" bestFit="1" width="30.5703125" customWidth="1"/>
-    <col min="17" max="18" bestFit="1" width="37.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="37.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75">
+    <row r="1" spans="1:22" ht="15.75">
       <c r="A1" s="176" t="s">
         <v>32</v>
       </c>
@@ -4629,7 +4612,7 @@
       <c r="S1" s="174"/>
       <c r="T1" s="175"/>
     </row>
-    <row r="2" ht="15.75">
+    <row r="2" spans="1:22" ht="15.75">
       <c r="A2" s="177"/>
       <c r="B2" s="179"/>
       <c r="C2" s="89" t="s">
@@ -4687,7 +4670,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:22">
       <c r="A3" s="14"/>
       <c r="B3" s="2"/>
       <c r="C3" s="140">
@@ -4695,7 +4678,7 @@
         <v>0.3</v>
       </c>
       <c r="D3" s="31">
-        <f ref="D3:M3" t="shared" si="0">IF(D38=0,$A$23,IF(D38=1,$A$24,IF(D38=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="D3:M3" si="0">IF(D38=0,$A$23,IF(D38=1,$A$24,IF(D38=2,$A$25,$A$26)))</f>
         <v>0.3</v>
       </c>
       <c r="E3" s="32">
@@ -4756,11 +4739,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:22">
       <c r="A4" s="15"/>
       <c r="B4" s="1"/>
       <c r="C4" s="141">
-        <f ref="C4:M4" t="shared" si="1">IF(C39=0,$A$23,IF(C39=1,$A$24,IF(C39=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C4:M4" si="1">IF(C39=0,$A$23,IF(C39=1,$A$24,IF(C39=2,$A$25,$A$26)))</f>
         <v>0</v>
       </c>
       <c r="D4" s="39">
@@ -4825,11 +4808,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:22">
       <c r="A5" s="148"/>
       <c r="B5" s="1"/>
       <c r="C5" s="141">
-        <f ref="C5:K5" t="shared" si="2">IF(C40=0,$A$23,IF(C40=1,$A$24,IF(C40=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C5:K5" si="2">IF(C40=0,$A$23,IF(C40=1,$A$24,IF(C40=2,$A$25,$A$26)))</f>
         <v>0.3</v>
       </c>
       <c r="D5" s="39">
@@ -4887,11 +4870,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:22">
       <c r="A6" s="148"/>
       <c r="B6" s="1"/>
       <c r="C6" s="141">
-        <f ref="C6:M6" t="shared" si="3">IF(C41=0,$A$23,IF(C41=1,$A$24,IF(C41=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C6:M6" si="3">IF(C41=0,$A$23,IF(C41=1,$A$24,IF(C41=2,$A$25,$A$26)))</f>
         <v>0.5</v>
       </c>
       <c r="D6" s="39">
@@ -4956,11 +4939,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:22">
       <c r="A7" s="79"/>
       <c r="B7" s="1"/>
       <c r="C7" s="141">
-        <f ref="C7:M7" t="shared" si="4">IF(C42=0,$A$23,IF(C42=1,$A$24,IF(C42=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C7:M7" si="4">IF(C42=0,$A$23,IF(C42=1,$A$24,IF(C42=2,$A$25,$A$26)))</f>
         <v>0.5</v>
       </c>
       <c r="D7" s="39">
@@ -5025,11 +5008,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:22">
       <c r="A8" s="148"/>
       <c r="B8" s="1"/>
       <c r="C8" s="141">
-        <f ref="C8:M8" t="shared" si="5">IF(C43=0,$A$23,IF(C43=1,$A$24,IF(C43=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C8:M8" si="5">IF(C43=0,$A$23,IF(C43=1,$A$24,IF(C43=2,$A$25,$A$26)))</f>
         <v>0</v>
       </c>
       <c r="D8" s="39">
@@ -5094,11 +5077,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" ht="15.75">
+    <row r="9" spans="1:22" ht="15.75">
       <c r="A9" s="147"/>
       <c r="B9" s="3"/>
       <c r="C9" s="142">
-        <f ref="C9:M9" t="shared" si="6">IF(C44=0,$A$23,IF(C44=1,$A$24,IF(C44=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C9:M9" si="6">IF(C44=0,$A$23,IF(C44=1,$A$24,IF(C44=2,$A$25,$A$26)))</f>
         <v>0</v>
       </c>
       <c r="D9" s="47">
@@ -5163,11 +5146,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:22">
       <c r="A10" s="149"/>
       <c r="B10" s="2"/>
       <c r="C10" s="140">
-        <f ref="C10:M10" t="shared" si="7">IF(C45=0,$A$23,IF(C45=1,$A$24,IF(C45=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C10:M10" si="7">IF(C45=0,$A$23,IF(C45=1,$A$24,IF(C45=2,$A$25,$A$26)))</f>
         <v>0.3</v>
       </c>
       <c r="D10" s="54">
@@ -5232,11 +5215,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:22">
       <c r="A11" s="15"/>
       <c r="B11" s="1"/>
       <c r="C11" s="141">
-        <f ref="C11:J11" t="shared" si="8">IF(C46=0,$A$23,IF(C46=1,$A$24,IF(C46=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C11:J11" si="8">IF(C46=0,$A$23,IF(C46=1,$A$24,IF(C46=2,$A$25,$A$26)))</f>
         <v>0.5</v>
       </c>
       <c r="D11" s="39">
@@ -5297,11 +5280,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:22">
       <c r="A12" s="148"/>
       <c r="B12" s="1"/>
       <c r="C12" s="141">
-        <f ref="C12:M12" t="shared" si="9">IF(C47=0,$A$23,IF(C47=1,$A$24,IF(C47=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C12:M12" si="9">IF(C47=0,$A$23,IF(C47=1,$A$24,IF(C47=2,$A$25,$A$26)))</f>
         <v>0.3</v>
       </c>
       <c r="D12" s="39">
@@ -5362,11 +5345,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:22">
       <c r="A13" s="15"/>
       <c r="B13" s="1"/>
       <c r="C13" s="141">
-        <f ref="C13:M13" t="shared" si="10">IF(C48=0,$A$23,IF(C48=1,$A$24,IF(C48=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C13:M13" si="10">IF(C48=0,$A$23,IF(C48=1,$A$24,IF(C48=2,$A$25,$A$26)))</f>
         <v>0.5</v>
       </c>
       <c r="D13" s="39">
@@ -5430,11 +5413,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" ht="15.75">
+    <row r="14" spans="1:22" ht="15.75">
       <c r="A14" s="16"/>
       <c r="B14" s="3"/>
       <c r="C14" s="142">
-        <f ref="C14:M14" t="shared" si="11">IF(C49=0,$A$23,IF(C49=1,$A$24,IF(C49=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C14:M14" si="11">IF(C49=0,$A$23,IF(C49=1,$A$24,IF(C49=2,$A$25,$A$26)))</f>
         <v>0.5</v>
       </c>
       <c r="D14" s="47">
@@ -5497,11 +5480,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:22">
       <c r="A15" s="149"/>
       <c r="B15" s="2"/>
       <c r="C15" s="140">
-        <f ref="C15:M15" t="shared" si="12">IF(C50=0,$A$23,IF(C50=1,$A$24,IF(C50=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C15:M15" si="12">IF(C50=0,$A$23,IF(C50=1,$A$24,IF(C50=2,$A$25,$A$26)))</f>
         <v>0</v>
       </c>
       <c r="D15" s="54">
@@ -5566,11 +5549,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:22">
       <c r="A16" s="15"/>
       <c r="B16" s="1"/>
       <c r="C16" s="141">
-        <f ref="C16:M16" t="shared" si="13">IF(C51=0,$A$23,IF(C51=1,$A$24,IF(C51=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C16:M16" si="13">IF(C51=0,$A$23,IF(C51=1,$A$24,IF(C51=2,$A$25,$A$26)))</f>
         <v>0</v>
       </c>
       <c r="D16" s="39">
@@ -5631,11 +5614,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" ht="15.75">
+    <row r="17" spans="1:22" ht="15.75">
       <c r="A17" s="129"/>
       <c r="B17" s="3"/>
       <c r="C17" s="142">
-        <f ref="C17:M17" t="shared" si="14">IF(C52=0,$A$23,IF(C52=1,$A$24,IF(C52=2,$A$25,$A$26)))</f>
+        <f t="shared" ref="C17:M17" si="14">IF(C52=0,$A$23,IF(C52=1,$A$24,IF(C52=2,$A$25,$A$26)))</f>
         <v>0.5</v>
       </c>
       <c r="D17" s="47">
@@ -5700,104 +5683,104 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19">
-      <c r="H19" s="0" t="s">
+    <row r="19" spans="1:22">
+      <c r="H19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20">
-      <c r="K20" s="0" t="s">
+    <row r="20" spans="1:22">
+      <c r="K20" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="0" t="s">
+      <c r="L20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21">
-      <c r="E21" s="0" t="s">
+    <row r="21" spans="1:22">
+      <c r="E21" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="0" t="s">
+      <c r="J21" t="s">
         <v>31</v>
       </c>
-      <c r="L21" s="0" t="s">
+      <c r="L21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:22">
       <c r="A22" s="125" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="125" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" t="s">
         <v>31</v>
       </c>
       <c r="H22" s="130"/>
-      <c r="J22" s="0" t="s">
+      <c r="J22" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="0" t="s">
+      <c r="K22" t="s">
         <v>31</v>
       </c>
-      <c r="L22" s="0" t="s">
+      <c r="L22" t="s">
         <v>31</v>
       </c>
-      <c r="Q22" s="0" t="s">
+      <c r="Q22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:22">
       <c r="A23" s="80">
         <v>0</v>
       </c>
       <c r="B23" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" t="s">
         <v>31</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="G23" t="s">
         <v>31</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="H23" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="I23" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="0" t="s">
+      <c r="K23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:22">
       <c r="A24" s="80">
         <v>0.2</v>
       </c>
       <c r="B24" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="G24" t="s">
         <v>31</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="I24" t="s">
         <v>31</v>
       </c>
-      <c r="J24" s="0" t="s">
+      <c r="J24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:22">
       <c r="A25" s="80">
         <v>0.3</v>
       </c>
@@ -5805,42 +5788,42 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:22">
       <c r="A26" s="80">
         <v>0.5</v>
       </c>
       <c r="B26" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="0" t="s">
+      <c r="G26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27">
-      <c r="D27" s="0" t="s">
+    <row r="27" spans="1:22">
+      <c r="D27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28">
-      <c r="B28" s="0" t="s">
+    <row r="28" spans="1:22">
+      <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="H28" s="0" t="s">
+      <c r="H28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29">
-      <c r="F29" s="0" t="s">
+    <row r="29" spans="1:22">
+      <c r="F29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33">
-      <c r="F33" s="0" t="s">
+    <row r="33" spans="1:18">
+      <c r="F33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" ht="15.75"/>
-    <row r="36" ht="15.75">
+    <row r="35" spans="1:18" ht="15.75"/>
+    <row r="36" spans="1:18" ht="15.75">
       <c r="A36" s="176" t="s">
         <v>32</v>
       </c>
@@ -5868,7 +5851,7 @@
       <c r="Q36" s="184"/>
       <c r="R36" s="185"/>
     </row>
-    <row r="37" ht="15.75">
+    <row r="37" spans="1:18" ht="15.75">
       <c r="A37" s="177"/>
       <c r="B37" s="179"/>
       <c r="C37" s="89" t="s">
@@ -5920,7 +5903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:18">
       <c r="A38" s="18"/>
       <c r="B38" s="2"/>
       <c r="C38" s="140">
@@ -5968,7 +5951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:18">
       <c r="A39" s="17"/>
       <c r="B39" s="1"/>
       <c r="C39" s="141">
@@ -6016,7 +5999,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:18">
       <c r="A40" s="126"/>
       <c r="B40" s="1"/>
       <c r="C40" s="141">
@@ -6062,7 +6045,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:18">
       <c r="A41" s="126"/>
       <c r="B41" s="1"/>
       <c r="C41" s="141">
@@ -6110,7 +6093,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:18">
       <c r="A42" s="126"/>
       <c r="B42" s="1"/>
       <c r="C42" s="141">
@@ -6156,7 +6139,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:18">
       <c r="A43" s="126"/>
       <c r="B43" s="1"/>
       <c r="C43" s="141">
@@ -6202,7 +6185,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" ht="15.75">
+    <row r="44" spans="1:18" ht="15.75">
       <c r="A44" s="146"/>
       <c r="B44" s="3"/>
       <c r="C44" s="142">
@@ -6246,7 +6229,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:18">
       <c r="A45" s="18"/>
       <c r="B45" s="2"/>
       <c r="C45" s="140">
@@ -6294,7 +6277,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:18">
       <c r="A46" s="17"/>
       <c r="B46" s="1"/>
       <c r="C46" s="141">
@@ -6346,7 +6329,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:18">
       <c r="A47" s="17"/>
       <c r="B47" s="1"/>
       <c r="C47" s="141">
@@ -6396,7 +6379,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:18">
       <c r="A48" s="17"/>
       <c r="B48" s="1"/>
       <c r="C48" s="141">
@@ -6446,7 +6429,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" ht="15.75">
+    <row r="49" spans="1:18" ht="15.75">
       <c r="A49" s="19"/>
       <c r="B49" s="3"/>
       <c r="C49" s="142">
@@ -6494,7 +6477,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:18">
       <c r="A50" s="18"/>
       <c r="B50" s="2"/>
       <c r="C50" s="140">
@@ -6542,7 +6525,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:18">
       <c r="A51" s="17"/>
       <c r="B51" s="1"/>
       <c r="C51" s="141">
@@ -6592,7 +6575,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" ht="15.75">
+    <row r="52" spans="1:18" ht="15.75">
       <c r="A52" s="127"/>
       <c r="B52" s="3"/>
       <c r="C52" s="142">
@@ -6638,23 +6621,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55">
-      <c r="G55" s="0" t="s">
+    <row r="55" spans="1:18">
+      <c r="G55" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:18">
       <c r="A57" s="125" t="s">
         <v>59</v>
       </c>
       <c r="B57" s="125" t="s">
         <v>53</v>
       </c>
-      <c r="R57" s="0" t="s">
+      <c r="R57" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:18">
       <c r="A58" s="80">
         <v>0</v>
       </c>
@@ -6662,7 +6645,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:18">
       <c r="A59" s="80">
         <v>1</v>
       </c>
@@ -6670,7 +6653,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:18">
       <c r="A60" s="80">
         <v>2</v>
       </c>
@@ -6678,7 +6661,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:18">
       <c r="A61" s="80">
         <v>3</v>
       </c>
@@ -6687,7 +6670,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="8">
     <mergeCell ref="O1:T1"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="B36:B37"/>
@@ -6698,27 +6681,26 @@
     <mergeCell ref="N36:R36"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:M17">
-    <cfRule type="cellIs" dxfId="0" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="26" operator="greaterThan">
       <formula>0.09</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:T17">
-    <cfRule type="cellIs" dxfId="0" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="25" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C52">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:M52">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
   <ignoredErrors>
     <ignoredError sqref="C18:D18 E18:K18 L18:M18" formula="1"/>
   </ignoredErrors>
@@ -6738,16 +6720,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="50" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" customWidth="1"/>
     <col min="14" max="14" width="7.7109375" customWidth="1"/>
     <col min="18" max="19" width="7.7109375" customWidth="1"/>
     <col min="21" max="21" width="7.7109375" customWidth="1"/>
-    <col min="58" max="58" bestFit="1" width="9.5703125" customWidth="1"/>
+    <col min="58" max="58" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:68">
       <c r="A1" s="166" t="s">
         <v>32</v>
       </c>
@@ -6833,7 +6815,7 @@
       <c r="BO1" s="158"/>
       <c r="BP1" s="159"/>
     </row>
-    <row r="2" ht="15.75">
+    <row r="2" spans="1:68" ht="15.75">
       <c r="A2" s="167"/>
       <c r="B2" s="169"/>
       <c r="C2" s="69" t="s">
@@ -7035,7 +7017,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" ht="15.75">
+    <row r="3" spans="1:68" ht="15.75">
       <c r="A3" s="14"/>
       <c r="B3" s="2"/>
       <c r="C3" s="140">
@@ -7143,27 +7125,27 @@
       </c>
       <c r="BF3" s="26">
         <f>AVERAGE(C3,N3,Y3,AJ3,AU3)</f>
-        <v>77.21</v>
+        <v>77.209999999999994</v>
       </c>
       <c r="BG3" s="26">
-        <f ref="BG3:BP16" t="shared" si="0">AVERAGE(D3,O3,Z3,AK3,AV3)</f>
-        <v>77.21</v>
+        <f t="shared" ref="BG3:BP16" si="0">AVERAGE(D3,O3,Z3,AK3,AV3)</f>
+        <v>77.209999999999994</v>
       </c>
       <c r="BH3" s="26">
         <f t="shared" si="0"/>
-        <v>77.21</v>
+        <v>77.209999999999994</v>
       </c>
       <c r="BI3" s="26">
         <f t="shared" si="0"/>
-        <v>77.21</v>
+        <v>77.209999999999994</v>
       </c>
       <c r="BJ3" s="26">
         <f t="shared" si="0"/>
-        <v>77.21</v>
+        <v>77.209999999999994</v>
       </c>
       <c r="BK3" s="26">
         <f t="shared" si="0"/>
-        <v>77.21</v>
+        <v>77.209999999999994</v>
       </c>
       <c r="BL3" s="26">
         <v>0</v>
@@ -7176,14 +7158,14 @@
       </c>
       <c r="BO3" s="26">
         <f t="shared" si="0"/>
-        <v>77.21</v>
+        <v>77.209999999999994</v>
       </c>
       <c r="BP3" s="26">
         <f t="shared" si="0"/>
-        <v>77.21</v>
+        <v>77.209999999999994</v>
       </c>
     </row>
-    <row r="4" ht="15.75">
+    <row r="4" spans="1:68" ht="15.75">
       <c r="A4" s="15"/>
       <c r="B4" s="1"/>
       <c r="C4" s="141"/>
@@ -7296,7 +7278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" ht="15.75">
+    <row r="5" spans="1:68" ht="15.75">
       <c r="A5" s="148"/>
       <c r="B5" s="1"/>
       <c r="C5" s="141"/>
@@ -7383,7 +7365,7 @@
         <v>56</v>
       </c>
       <c r="BF5" s="26">
-        <f ref="BF5:BF14" t="shared" si="1">AVERAGE(C5,N5,Y5,AJ5,AU5)</f>
+        <f t="shared" ref="BF5:BF14" si="1">AVERAGE(C5,N5,Y5,AJ5,AU5)</f>
         <v>69.5</v>
       </c>
       <c r="BG5" s="26">
@@ -7409,7 +7391,7 @@
         <v>0</v>
       </c>
       <c r="BM5" s="26">
-        <f ref="BM5:BN16" t="shared" si="2">AVERAGE(J5,U5,AF5,AQ5,BB5)</f>
+        <f t="shared" ref="BM5:BN16" si="2">AVERAGE(J5,U5,AF5,AQ5,BB5)</f>
         <v>68</v>
       </c>
       <c r="BN5" s="26">
@@ -7423,22 +7405,22 @@
         <v>64.5</v>
       </c>
     </row>
-    <row r="6" ht="15.75">
+    <row r="6" spans="1:68" ht="15.75">
       <c r="A6" s="148"/>
       <c r="B6" s="1"/>
       <c r="C6" s="141">
-        <v>70.9</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="D6" s="39"/>
       <c r="E6" s="37"/>
       <c r="F6" s="37">
-        <v>70.9</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="G6" s="37">
-        <v>70.9</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="H6" s="37">
-        <v>70.9</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="I6" s="37"/>
       <c r="J6" s="37"/>
@@ -7507,7 +7489,7 @@
       <c r="BE6" s="40"/>
       <c r="BF6" s="26">
         <f t="shared" si="1"/>
-        <v>69.47000000000001</v>
+        <v>69.470000000000013</v>
       </c>
       <c r="BG6" s="26">
         <v>0</v>
@@ -7517,15 +7499,15 @@
       </c>
       <c r="BI6" s="26">
         <f t="shared" si="0"/>
-        <v>69.47000000000001</v>
+        <v>69.470000000000013</v>
       </c>
       <c r="BJ6" s="26">
         <f t="shared" si="0"/>
-        <v>69.47000000000001</v>
+        <v>69.470000000000013</v>
       </c>
       <c r="BK6" s="26">
         <f t="shared" si="0"/>
-        <v>69.47000000000001</v>
+        <v>69.470000000000013</v>
       </c>
       <c r="BL6" s="26">
         <v>0</v>
@@ -7543,7 +7525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" ht="15.75">
+    <row r="7" spans="1:68" ht="15.75">
       <c r="A7" s="79"/>
       <c r="B7" s="1"/>
       <c r="C7" s="141"/>
@@ -7635,7 +7617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" ht="15.75">
+    <row r="8" spans="1:68" ht="15.75">
       <c r="A8" s="148"/>
       <c r="B8" s="1"/>
       <c r="C8" s="141"/>
@@ -7716,7 +7698,7 @@
         <v>0</v>
       </c>
       <c r="BL8" s="26">
-        <f ref="BL8:BL16" t="shared" si="3">AVERAGE(I8,T8,AE8,AP8,BA8)</f>
+        <f t="shared" ref="BL8:BL16" si="3">AVERAGE(I8,T8,AE8,AP8,BA8)</f>
         <v>83.39</v>
       </c>
       <c r="BM8" s="26">
@@ -7732,7 +7714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" ht="15.75">
+    <row r="9" spans="1:68" ht="15.75">
       <c r="A9" s="147"/>
       <c r="B9" s="3"/>
       <c r="C9" s="142"/>
@@ -7827,7 +7809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" ht="15.75">
+    <row r="10" spans="1:68" ht="15.75">
       <c r="A10" s="149"/>
       <c r="B10" s="2"/>
       <c r="C10" s="140">
@@ -7929,14 +7911,14 @@
         <v>0</v>
       </c>
       <c r="BO10" s="26">
-        <f ref="BO10:BO16" t="shared" si="4">AVERAGE(L10,W10,AH10,AS10,BD10)</f>
+        <f t="shared" ref="BO10:BO16" si="4">AVERAGE(L10,W10,AH10,AS10,BD10)</f>
         <v>0</v>
       </c>
       <c r="BP10" s="26">
         <v>0</v>
       </c>
     </row>
-    <row r="11" ht="15.75">
+    <row r="11" spans="1:68" ht="15.75">
       <c r="A11" s="15"/>
       <c r="B11" s="1"/>
       <c r="C11" s="141"/>
@@ -7994,7 +7976,7 @@
         <v>82.4</v>
       </c>
       <c r="AK11" s="37">
-        <v>78.96</v>
+        <v>78.959999999999994</v>
       </c>
       <c r="AL11" s="37">
         <v>90.36</v>
@@ -8030,11 +8012,11 @@
       <c r="BE11" s="40"/>
       <c r="BF11" s="26">
         <f t="shared" si="1"/>
-        <v>90.065</v>
+        <v>90.064999999999998</v>
       </c>
       <c r="BG11" s="26">
         <f t="shared" si="0"/>
-        <v>58.89666666666667</v>
+        <v>58.896666666666668</v>
       </c>
       <c r="BH11" s="26">
         <f t="shared" si="0"/>
@@ -8042,7 +8024,7 @@
       </c>
       <c r="BI11" s="26">
         <f t="shared" si="0"/>
-        <v>97.13499999999999</v>
+        <v>97.134999999999991</v>
       </c>
       <c r="BJ11" s="26">
         <f t="shared" si="0"/>
@@ -8050,7 +8032,7 @@
       </c>
       <c r="BK11" s="26">
         <f t="shared" si="0"/>
-        <v>43.48666666666667</v>
+        <v>43.486666666666672</v>
       </c>
       <c r="BL11" s="26">
         <v>0</v>
@@ -8069,7 +8051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" ht="15.75">
+    <row r="12" spans="1:68" ht="15.75">
       <c r="A12" s="148"/>
       <c r="B12" s="1"/>
       <c r="C12" s="141">
@@ -8177,7 +8159,7 @@
       </c>
       <c r="BI12" s="26">
         <f t="shared" si="0"/>
-        <v>54.38249999999999</v>
+        <v>54.382499999999993</v>
       </c>
       <c r="BJ12" s="26">
         <f t="shared" si="0"/>
@@ -8203,7 +8185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" ht="15.75">
+    <row r="13" spans="1:68" ht="15.75">
       <c r="A13" s="15"/>
       <c r="B13" s="1"/>
       <c r="C13" s="141">
@@ -8295,19 +8277,19 @@
       <c r="BE13" s="40"/>
       <c r="BF13" s="26">
         <f t="shared" si="1"/>
-        <v>62.3525</v>
+        <v>62.352499999999999</v>
       </c>
       <c r="BG13" s="26">
         <f t="shared" si="0"/>
-        <v>62.3525</v>
+        <v>62.352499999999999</v>
       </c>
       <c r="BH13" s="26">
         <f t="shared" si="0"/>
-        <v>54.435</v>
+        <v>54.435000000000002</v>
       </c>
       <c r="BI13" s="26">
         <f t="shared" si="0"/>
-        <v>62.3525</v>
+        <v>62.352499999999999</v>
       </c>
       <c r="BJ13" s="26">
         <f t="shared" si="0"/>
@@ -8332,7 +8314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" ht="15.75">
+    <row r="14" spans="1:68" ht="15.75">
       <c r="A14" s="16"/>
       <c r="B14" s="3"/>
       <c r="C14" s="142"/>
@@ -8355,24 +8337,24 @@
       <c r="L14" s="45"/>
       <c r="M14" s="46"/>
       <c r="N14" s="140">
-        <v>20.06</v>
+        <v>20.059999999999999</v>
       </c>
       <c r="O14" s="54">
-        <v>20.06</v>
+        <v>20.059999999999999</v>
       </c>
       <c r="P14" s="49">
-        <v>20.06</v>
+        <v>20.059999999999999</v>
       </c>
       <c r="Q14" s="49">
-        <v>20.06</v>
+        <v>20.059999999999999</v>
       </c>
       <c r="R14" s="57">
-        <v>20.06</v>
+        <v>20.059999999999999</v>
       </c>
       <c r="S14" s="49"/>
       <c r="T14" s="49"/>
       <c r="U14" s="54">
-        <v>20.06</v>
+        <v>20.059999999999999</v>
       </c>
       <c r="V14" s="47"/>
       <c r="W14" s="45"/>
@@ -8399,7 +8381,7 @@
         <v>39.75</v>
       </c>
       <c r="AN14" s="45">
-        <v>32.48</v>
+        <v>32.479999999999997</v>
       </c>
       <c r="AO14" s="45"/>
       <c r="AP14" s="45"/>
@@ -8436,7 +8418,7 @@
       </c>
       <c r="BH14" s="26">
         <f t="shared" si="0"/>
-        <v>10.03</v>
+        <v>10.029999999999999</v>
       </c>
       <c r="BI14" s="26">
         <f t="shared" si="0"/>
@@ -8454,7 +8436,7 @@
       </c>
       <c r="BM14" s="26">
         <f t="shared" si="2"/>
-        <v>48.395</v>
+        <v>48.395000000000003</v>
       </c>
       <c r="BN14" s="26">
         <v>0</v>
@@ -8466,7 +8448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" ht="15.75">
+    <row r="15" spans="1:68" ht="15.75">
       <c r="A15" s="149"/>
       <c r="B15" s="2"/>
       <c r="C15" s="140"/>
@@ -8586,7 +8568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" ht="15.75">
+    <row r="16" spans="1:68" ht="15.75">
       <c r="A16" s="15"/>
       <c r="B16" s="1"/>
       <c r="C16" s="141"/>
@@ -8723,7 +8705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" ht="15.75">
+    <row r="17" spans="1:68" ht="15.75">
       <c r="A17" s="129"/>
       <c r="B17" s="3"/>
       <c r="C17" s="142"/>
@@ -8815,8 +8797,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" ht="15.75"/>
-    <row r="20" ht="15.75">
+    <row r="19" spans="1:68" ht="15.75"/>
+    <row r="20" spans="1:68" ht="15.75">
       <c r="A20" s="176" t="s">
         <v>32</v>
       </c>
@@ -8896,11 +8878,11 @@
       <c r="BJ20" s="174"/>
       <c r="BK20" s="174"/>
       <c r="BL20" s="175"/>
-      <c r="BP20" s="0" t="s">
+      <c r="BP20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" ht="15.75">
+    <row r="21" spans="1:68" ht="15.75">
       <c r="A21" s="177"/>
       <c r="B21" s="179"/>
       <c r="C21" s="89" t="s">
@@ -9090,7 +9072,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:68">
       <c r="A22" s="14"/>
       <c r="B22" s="2"/>
       <c r="C22" s="140">
@@ -9336,7 +9318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:68">
       <c r="A23" s="15"/>
       <c r="B23" s="1"/>
       <c r="C23" s="141">
@@ -9582,7 +9564,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:68">
       <c r="A24" s="148"/>
       <c r="B24" s="1"/>
       <c r="C24" s="141">
@@ -9828,7 +9810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:68">
       <c r="A25" s="148"/>
       <c r="B25" s="1"/>
       <c r="C25" s="141">
@@ -10074,7 +10056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:68">
       <c r="A26" s="79"/>
       <c r="B26" s="1"/>
       <c r="C26" s="141">
@@ -10320,7 +10302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:68">
       <c r="A27" s="148"/>
       <c r="B27" s="1"/>
       <c r="C27" s="141">
@@ -10566,7 +10548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" ht="15.75">
+    <row r="28" spans="1:68" ht="15.75">
       <c r="A28" s="147"/>
       <c r="B28" s="3"/>
       <c r="C28" s="142">
@@ -10789,7 +10771,7 @@
         <f>'PÇ Destekleme Oranları'!M9</f>
         <v>0</v>
       </c>
-      <c r="BF28" s="0" t="s">
+      <c r="BF28" t="s">
         <v>31</v>
       </c>
       <c r="BG28" s="86">
@@ -10815,7 +10797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:68">
       <c r="A29" s="149"/>
       <c r="B29" s="2"/>
       <c r="C29" s="140">
@@ -11061,7 +11043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:68">
       <c r="A30" s="15"/>
       <c r="B30" s="1"/>
       <c r="C30" s="141">
@@ -11307,7 +11289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:68">
       <c r="A31" s="79"/>
       <c r="B31" s="1"/>
       <c r="C31" s="141">
@@ -11553,7 +11535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:68">
       <c r="A32" s="15"/>
       <c r="B32" s="1"/>
       <c r="C32" s="141">
@@ -11799,7 +11781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" ht="15.75">
+    <row r="33" spans="1:70" ht="15.75">
       <c r="A33" s="16"/>
       <c r="B33" s="3"/>
       <c r="C33" s="142">
@@ -12045,7 +12027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:70">
       <c r="A34" s="149"/>
       <c r="B34" s="2"/>
       <c r="C34" s="140">
@@ -12290,11 +12272,11 @@
         <f>'PÇ Destekleme Oranları'!V15</f>
         <v>7</v>
       </c>
-      <c r="BP34" s="0" t="s">
+      <c r="BP34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:70">
       <c r="A35" s="15"/>
       <c r="B35" s="1"/>
       <c r="C35" s="141">
@@ -12540,7 +12522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" ht="15.75">
+    <row r="36" spans="1:70" ht="15.75">
       <c r="A36" s="129"/>
       <c r="B36" s="3"/>
       <c r="C36" s="142">
@@ -12786,8 +12768,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" ht="15.75"/>
-    <row r="39">
+    <row r="38" spans="1:70" ht="15.75"/>
+    <row r="39" spans="1:70">
       <c r="A39" s="166" t="s">
         <v>32</v>
       </c>
@@ -12873,7 +12855,7 @@
       <c r="BO39" s="158"/>
       <c r="BP39" s="159"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:70">
       <c r="A40" s="167"/>
       <c r="B40" s="169"/>
       <c r="C40" s="69" t="s">
@@ -13078,7 +13060,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:70">
       <c r="A41" s="14"/>
       <c r="B41" s="2"/>
       <c r="C41" s="143">
@@ -13086,20 +13068,20 @@
         <v>23.738999999999997</v>
       </c>
       <c r="D41" s="99">
-        <f ref="D41:M41" t="shared" si="5">D3*D22</f>
+        <f t="shared" ref="D41:M41" si="5">D3*D22</f>
         <v>23.738999999999997</v>
       </c>
       <c r="E41" s="100">
         <f t="shared" si="5"/>
-        <v>39.565</v>
+        <v>39.564999999999998</v>
       </c>
       <c r="F41" s="100">
         <f t="shared" si="5"/>
-        <v>39.565</v>
+        <v>39.564999999999998</v>
       </c>
       <c r="G41" s="100">
         <f t="shared" si="5"/>
-        <v>39.565</v>
+        <v>39.564999999999998</v>
       </c>
       <c r="H41" s="100">
         <f t="shared" si="5"/>
@@ -13126,11 +13108,11 @@
         <v>23.738999999999997</v>
       </c>
       <c r="N41" s="143">
-        <f ref="N41:BE41" t="shared" si="6">N3*N22</f>
+        <f t="shared" ref="N41:BE41" si="6">N3*N22</f>
         <v>0</v>
       </c>
       <c r="O41" s="99">
-        <f ref="O41:X41" t="shared" si="7">O3*O22</f>
+        <f t="shared" ref="O41:X41" si="7">O3*O22</f>
         <v>0</v>
       </c>
       <c r="P41" s="100">
@@ -13215,11 +13197,11 @@
       </c>
       <c r="AJ41" s="99">
         <f t="shared" si="6"/>
-        <v>20.886</v>
+        <v>20.885999999999999</v>
       </c>
       <c r="AK41" s="100">
         <f t="shared" si="6"/>
-        <v>20.886</v>
+        <v>20.885999999999999</v>
       </c>
       <c r="AL41" s="100">
         <f t="shared" si="6"/>
@@ -13235,7 +13217,7 @@
       </c>
       <c r="AO41" s="100">
         <f t="shared" si="6"/>
-        <v>20.886</v>
+        <v>20.885999999999999</v>
       </c>
       <c r="AP41" s="100">
         <f t="shared" si="6"/>
@@ -13251,11 +13233,11 @@
       </c>
       <c r="AS41" s="100">
         <f t="shared" si="6"/>
-        <v>20.886</v>
+        <v>20.885999999999999</v>
       </c>
       <c r="AT41" s="101">
         <f t="shared" si="6"/>
-        <v>20.886</v>
+        <v>20.885999999999999</v>
       </c>
       <c r="AU41" s="67">
         <f>AU3*AU22</f>
@@ -13303,27 +13285,27 @@
       </c>
       <c r="BF41" s="26">
         <f>(C41*$BG$22+N41*$BH$22+Y41*$BI$22+AJ41*$BJ$22+AU41*$BK$22)/SUM($BG$22:$BK$22)</f>
-        <v>20.65033333333333</v>
+        <v>20.650333333333329</v>
       </c>
       <c r="BG41" s="26">
-        <f ref="BG41:BP41" t="shared" si="8">(D41*$BG$22+O41*$BH$22+Z41*$BI$22+AK41*$BJ$22+AV41*$BK$22)/SUM($BG$22:$BK$22)</f>
-        <v>20.65033333333333</v>
+        <f t="shared" ref="BG41:BP41" si="8">(D41*$BG$22+O41*$BH$22+Z41*$BI$22+AK41*$BJ$22+AV41*$BK$22)/SUM($BG$22:$BK$22)</f>
+        <v>20.650333333333329</v>
       </c>
       <c r="BH41" s="26">
         <f t="shared" si="8"/>
-        <v>34.41722222222222</v>
+        <v>34.417222222222222</v>
       </c>
       <c r="BI41" s="26">
         <f t="shared" si="8"/>
-        <v>34.41722222222222</v>
+        <v>34.417222222222222</v>
       </c>
       <c r="BJ41" s="26">
         <f t="shared" si="8"/>
-        <v>34.41722222222222</v>
+        <v>34.417222222222222</v>
       </c>
       <c r="BK41" s="26">
         <f>(H41*$BG$22+S41*$BH$22+AD41*$BI$22+AO41*$BJ$22+AZ41*$BK$22)/SUM($BG$22:$BK$22)</f>
-        <v>20.65033333333333</v>
+        <v>20.650333333333329</v>
       </c>
       <c r="BL41" s="26">
         <f t="shared" si="8"/>
@@ -13339,21 +13321,21 @@
       </c>
       <c r="BO41" s="26">
         <f t="shared" si="8"/>
-        <v>20.65033333333333</v>
+        <v>20.650333333333329</v>
       </c>
       <c r="BP41" s="73">
         <f t="shared" si="8"/>
-        <v>20.65033333333333</v>
+        <v>20.650333333333329</v>
       </c>
       <c r="BR41" s="94">
         <v>3</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:70">
       <c r="A42" s="15"/>
       <c r="B42" s="1"/>
       <c r="C42" s="144">
-        <f ref="C42:BE42" t="shared" si="9">C4*C23</f>
+        <f t="shared" ref="C42:BE42" si="9">C4*C23</f>
         <v>0</v>
       </c>
       <c r="D42" s="108">
@@ -13402,15 +13384,15 @@
       </c>
       <c r="O42" s="108">
         <f t="shared" si="9"/>
-        <v>26.325</v>
+        <v>26.324999999999999</v>
       </c>
       <c r="P42" s="109">
         <f t="shared" si="9"/>
-        <v>26.325</v>
+        <v>26.324999999999999</v>
       </c>
       <c r="Q42" s="109">
         <f t="shared" si="9"/>
-        <v>26.325</v>
+        <v>26.324999999999999</v>
       </c>
       <c r="R42" s="111">
         <f t="shared" si="9"/>
@@ -13577,7 +13559,7 @@
         <v>0</v>
       </c>
       <c r="BG42" s="27">
-        <f ref="BG42:BP42" t="shared" si="10">(D42*$BG$23+O42*$BH$23+Z42*$BI$23+AK42*$BJ$23+AV42*$BK$23)/SUM($BG$23:$BK$23)</f>
+        <f t="shared" ref="BG42:BP42" si="10">(D42*$BG$23+O42*$BH$23+Z42*$BI$23+AK42*$BJ$23+AV42*$BK$23)/SUM($BG$23:$BK$23)</f>
         <v>24.328999999999997</v>
       </c>
       <c r="BH42" s="27">
@@ -13620,7 +13602,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:70">
       <c r="A43" s="148"/>
       <c r="B43" s="1"/>
       <c r="C43" s="144">
@@ -13628,7 +13610,7 @@
         <v>0</v>
       </c>
       <c r="D43" s="108">
-        <f ref="D43:BD43" t="shared" si="11">D5*D24</f>
+        <f t="shared" ref="D43:BD43" si="11">D5*D24</f>
         <v>0</v>
       </c>
       <c r="E43" s="109">
@@ -13801,7 +13783,7 @@
       </c>
       <c r="AU43" s="27">
         <f t="shared" si="11"/>
-        <v>18.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="AV43" s="109">
         <f t="shared" si="11"/>
@@ -13829,7 +13811,7 @@
       </c>
       <c r="BB43" s="109">
         <f t="shared" si="11"/>
-        <v>18.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="BC43" s="109">
         <f t="shared" si="11"/>
@@ -13848,8 +13830,8 @@
         <v>12.315</v>
       </c>
       <c r="BG43" s="27">
-        <f ref="BG43:BP43" t="shared" si="12">(D43*$BG$24+O43*$BH$24+Z43*$BI$24+AK43*$BJ$24+AV43*$BK$24)/SUM($BG$24:$BK$24)</f>
-        <v>12.825</v>
+        <f t="shared" ref="BG43:BP43" si="12">(D43*$BG$24+O43*$BH$24+Z43*$BI$24+AK43*$BJ$24+AV43*$BK$24)/SUM($BG$24:$BK$24)</f>
+        <v>12.824999999999999</v>
       </c>
       <c r="BH43" s="27">
         <f t="shared" si="12"/>
@@ -13857,11 +13839,11 @@
       </c>
       <c r="BI43" s="27">
         <f t="shared" si="12"/>
-        <v>24.175</v>
+        <v>24.175000000000001</v>
       </c>
       <c r="BJ43" s="27">
         <f t="shared" si="12"/>
-        <v>24.175</v>
+        <v>24.175000000000001</v>
       </c>
       <c r="BK43" s="27">
         <f t="shared" si="12"/>
@@ -13885,18 +13867,18 @@
       </c>
       <c r="BP43" s="74">
         <f t="shared" si="12"/>
-        <v>18.925</v>
+        <v>18.925000000000001</v>
       </c>
       <c r="BR43" s="94">
         <v>5</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:70">
       <c r="A44" s="148"/>
       <c r="B44" s="1"/>
       <c r="C44" s="144">
-        <f ref="C44:BE44" t="shared" si="13">C6*C25</f>
-        <v>35.45</v>
+        <f t="shared" ref="C44:BE44" si="13">C6*C25</f>
+        <v>35.450000000000003</v>
       </c>
       <c r="D44" s="108">
         <f t="shared" si="13"/>
@@ -13908,15 +13890,15 @@
       </c>
       <c r="F44" s="109">
         <f t="shared" si="13"/>
-        <v>35.45</v>
+        <v>35.450000000000003</v>
       </c>
       <c r="G44" s="109">
         <f t="shared" si="13"/>
-        <v>35.45</v>
+        <v>35.450000000000003</v>
       </c>
       <c r="H44" s="109">
         <f t="shared" si="13"/>
-        <v>35.45</v>
+        <v>35.450000000000003</v>
       </c>
       <c r="I44" s="109">
         <f t="shared" si="13"/>
@@ -14028,7 +14010,7 @@
       </c>
       <c r="AJ44" s="108">
         <f t="shared" si="13"/>
-        <v>30.935</v>
+        <v>30.934999999999999</v>
       </c>
       <c r="AK44" s="109">
         <f t="shared" si="13"/>
@@ -14040,15 +14022,15 @@
       </c>
       <c r="AM44" s="109">
         <f t="shared" si="13"/>
-        <v>30.935</v>
+        <v>30.934999999999999</v>
       </c>
       <c r="AN44" s="109">
         <f t="shared" si="13"/>
-        <v>30.935</v>
+        <v>30.934999999999999</v>
       </c>
       <c r="AO44" s="109">
         <f t="shared" si="13"/>
-        <v>30.935</v>
+        <v>30.934999999999999</v>
       </c>
       <c r="AP44" s="109">
         <f t="shared" si="13"/>
@@ -14119,7 +14101,7 @@
         <v>34.484750000000005</v>
       </c>
       <c r="BG44" s="27">
-        <f ref="BG44:BP44" t="shared" si="14">(D44*$BG$25+O44*$BH$25+Z44*$BI$25+AK44*$BJ$25+AV44*$BK$25)/SUM($BG$25:$BK$25)</f>
+        <f t="shared" ref="BG44:BP44" si="14">(D44*$BG$25+O44*$BH$25+Z44*$BI$25+AK44*$BJ$25+AV44*$BK$25)/SUM($BG$25:$BK$25)</f>
         <v>0</v>
       </c>
       <c r="BH44" s="27">
@@ -14162,11 +14144,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:70">
       <c r="A45" s="79"/>
       <c r="B45" s="1"/>
       <c r="C45" s="144">
-        <f ref="C45:BE45" t="shared" si="15">C7*C26</f>
+        <f t="shared" ref="C45:BE45" si="15">C7*C26</f>
         <v>0</v>
       </c>
       <c r="D45" s="108">
@@ -14390,7 +14372,7 @@
         <v>0</v>
       </c>
       <c r="BG45" s="67">
-        <f ref="BG45:BP45" t="shared" si="16">(D45*$BG$26+O45*$BH$26+Z45*$BI$26+AK45*$BJ$26+AV45*$BK$26)/SUM($BG$26:$BK$26)</f>
+        <f t="shared" ref="BG45:BP45" si="16">(D45*$BG$26+O45*$BH$26+Z45*$BI$26+AK45*$BJ$26+AV45*$BK$26)/SUM($BG$26:$BK$26)</f>
         <v>0</v>
       </c>
       <c r="BH45" s="67">
@@ -14433,11 +14415,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:70">
       <c r="A46" s="148"/>
       <c r="B46" s="1"/>
       <c r="C46" s="144">
-        <f ref="C46:BE46" t="shared" si="17">C8*C27</f>
+        <f t="shared" ref="C46:BE46" si="17">C8*C27</f>
         <v>0</v>
       </c>
       <c r="D46" s="108">
@@ -14661,7 +14643,7 @@
         <v>0</v>
       </c>
       <c r="BG46" s="27">
-        <f ref="BG46:BP46" t="shared" si="18">(D46*$BG$27+O46*$BH$27+Z46*$BI$27+AK46*$BJ$27+AV46*$BK$27)/SUM($BG$27:$BK$27)</f>
+        <f t="shared" ref="BG46:BP46" si="18">(D46*$BG$27+O46*$BH$27+Z46*$BI$27+AK46*$BJ$27+AV46*$BK$27)/SUM($BG$27:$BK$27)</f>
         <v>0</v>
       </c>
       <c r="BH46" s="27">
@@ -14704,11 +14686,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:70">
       <c r="A47" s="147"/>
       <c r="B47" s="3"/>
       <c r="C47" s="145">
-        <f ref="C47:BE47" t="shared" si="19">C9*C28</f>
+        <f t="shared" ref="C47:BE47" si="19">C9*C28</f>
         <v>0</v>
       </c>
       <c r="D47" s="116">
@@ -14909,7 +14891,7 @@
       </c>
       <c r="BA47" s="117">
         <f>BA9*BA28</f>
-        <v>40.065</v>
+        <v>40.064999999999998</v>
       </c>
       <c r="BB47" s="117">
         <f t="shared" si="19"/>
@@ -14932,7 +14914,7 @@
         <v>0</v>
       </c>
       <c r="BG47" s="72">
-        <f ref="BG47:BP47" t="shared" si="20">(D47*$BG$28+O47*$BH$28+Z47*$BI$28+AK47*$BJ$28+AV47*$BK$28)/SUM($BG$28:$BK$28)</f>
+        <f t="shared" ref="BG47:BP47" si="20">(D47*$BG$28+O47*$BH$28+Z47*$BI$28+AK47*$BJ$28+AV47*$BK$28)/SUM($BG$28:$BK$28)</f>
         <v>0</v>
       </c>
       <c r="BH47" s="72">
@@ -14975,7 +14957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:70">
       <c r="A48" s="149"/>
       <c r="B48" s="2"/>
       <c r="C48" s="103">
@@ -14983,7 +14965,7 @@
         <v>0</v>
       </c>
       <c r="D48" s="103">
-        <f ref="D48:BE48" t="shared" si="21">D10*D29</f>
+        <f t="shared" ref="D48:BE48" si="21">D10*D29</f>
         <v>0</v>
       </c>
       <c r="E48" s="103">
@@ -15203,7 +15185,7 @@
         <v>0</v>
       </c>
       <c r="BG48" s="26">
-        <f ref="BG48:BP48" t="shared" si="22">(D48*$BG$29+O48*$BH$29+Z48*$BI$29+AK48*$BJ$29+AV48*$BK$29)/SUM($BG$29:$BK$29)</f>
+        <f t="shared" ref="BG48:BP48" si="22">(D48*$BG$29+O48*$BH$29+Z48*$BI$29+AK48*$BJ$29+AV48*$BK$29)/SUM($BG$29:$BK$29)</f>
         <v>0</v>
       </c>
       <c r="BH48" s="26">
@@ -15246,11 +15228,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:70">
       <c r="A49" s="15"/>
       <c r="B49" s="1"/>
       <c r="C49" s="144">
-        <f ref="C49:BE49" t="shared" si="23">C11*C30</f>
+        <f t="shared" ref="C49:BE49" si="23">C11*C30</f>
         <v>0</v>
       </c>
       <c r="D49" s="108">
@@ -15311,11 +15293,11 @@
       </c>
       <c r="R49" s="111">
         <f t="shared" si="23"/>
-        <v>19.569</v>
+        <v>19.568999999999999</v>
       </c>
       <c r="S49" s="109">
         <f t="shared" si="23"/>
-        <v>19.569</v>
+        <v>19.568999999999999</v>
       </c>
       <c r="T49" s="109">
         <f t="shared" si="23"/>
@@ -15355,11 +15337,11 @@
       </c>
       <c r="AC49" s="109">
         <f t="shared" si="23"/>
-        <v>19.569</v>
+        <v>19.568999999999999</v>
       </c>
       <c r="AD49" s="108">
         <f t="shared" si="23"/>
-        <v>19.569</v>
+        <v>19.568999999999999</v>
       </c>
       <c r="AE49" s="109">
         <f t="shared" si="23"/>
@@ -15387,15 +15369,15 @@
       </c>
       <c r="AK49" s="109">
         <f t="shared" si="23"/>
-        <v>23.688</v>
+        <v>23.687999999999999</v>
       </c>
       <c r="AL49" s="109">
         <f t="shared" si="23"/>
-        <v>18.072</v>
+        <v>18.071999999999999</v>
       </c>
       <c r="AM49" s="109">
         <f t="shared" si="23"/>
-        <v>49.165</v>
+        <v>49.164999999999999</v>
       </c>
       <c r="AN49" s="109">
         <f t="shared" si="23"/>
@@ -15427,11 +15409,11 @@
       </c>
       <c r="AU49" s="27">
         <f t="shared" si="23"/>
-        <v>48.865</v>
+        <v>48.865000000000002</v>
       </c>
       <c r="AV49" s="109">
         <f t="shared" si="23"/>
-        <v>29.319</v>
+        <v>29.318999999999999</v>
       </c>
       <c r="AW49" s="109">
         <f t="shared" si="23"/>
@@ -15471,11 +15453,11 @@
       </c>
       <c r="BF49" s="27">
         <f>(C49*$BG$30+N49*$BH$30+Y49*$BI$30+AJ49*$BJ$30+AU49*$BK$30)/SUM($BG$30:$BK$30)</f>
-        <v>32.28925</v>
+        <v>32.289250000000003</v>
       </c>
       <c r="BG49" s="27">
-        <f ref="BG49:BP49" t="shared" si="24">(D49*$BG$30+O49*$BH$30+Z49*$BI$30+AK49*$BJ$30+AV49*$BK$30)/SUM($BG$30:$BK$30)</f>
-        <v>19.11555</v>
+        <f t="shared" ref="BG49:BP49" si="24">(D49*$BG$30+O49*$BH$30+Z49*$BI$30+AK49*$BJ$30+AV49*$BK$30)/SUM($BG$30:$BK$30)</f>
+        <v>19.115549999999999</v>
       </c>
       <c r="BH49" s="27">
         <f t="shared" si="24"/>
@@ -15483,7 +15465,7 @@
       </c>
       <c r="BI49" s="27">
         <f t="shared" si="24"/>
-        <v>33.87775</v>
+        <v>33.877749999999999</v>
       </c>
       <c r="BJ49" s="27">
         <f t="shared" si="24"/>
@@ -15517,16 +15499,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:70">
       <c r="A50" s="79"/>
       <c r="B50" s="1"/>
       <c r="C50" s="144">
-        <f ref="C50:BE50" t="shared" si="25">C12*C31</f>
-        <v>16.329</v>
+        <f t="shared" ref="C50:BE50" si="25">C12*C31</f>
+        <v>16.329000000000001</v>
       </c>
       <c r="D50" s="108">
         <f t="shared" si="25"/>
-        <v>16.329</v>
+        <v>16.329000000000001</v>
       </c>
       <c r="E50" s="109">
         <f t="shared" si="25"/>
@@ -15534,11 +15516,11 @@
       </c>
       <c r="F50" s="109">
         <f t="shared" si="25"/>
-        <v>16.329</v>
+        <v>16.329000000000001</v>
       </c>
       <c r="G50" s="109">
         <f t="shared" si="25"/>
-        <v>16.329</v>
+        <v>16.329000000000001</v>
       </c>
       <c r="H50" s="109">
         <f t="shared" si="25"/>
@@ -15566,11 +15548,11 @@
       </c>
       <c r="N50" s="144">
         <f t="shared" si="25"/>
-        <v>17.424</v>
+        <v>17.423999999999999</v>
       </c>
       <c r="O50" s="108">
         <f t="shared" si="25"/>
-        <v>17.424</v>
+        <v>17.423999999999999</v>
       </c>
       <c r="P50" s="109">
         <f t="shared" si="25"/>
@@ -15578,11 +15560,11 @@
       </c>
       <c r="Q50" s="109">
         <f t="shared" si="25"/>
-        <v>17.424</v>
+        <v>17.423999999999999</v>
       </c>
       <c r="R50" s="111">
         <f t="shared" si="25"/>
-        <v>17.424</v>
+        <v>17.423999999999999</v>
       </c>
       <c r="S50" s="109">
         <f t="shared" si="25"/>
@@ -15710,7 +15692,7 @@
       </c>
       <c r="AX50" s="109">
         <f t="shared" si="25"/>
-        <v>16.389</v>
+        <v>16.388999999999999</v>
       </c>
       <c r="AY50" s="109">
         <f t="shared" si="25"/>
@@ -15742,23 +15724,23 @@
       </c>
       <c r="BF50" s="27">
         <f>(C50*$BG$31+N50*$BH$31+Y50*$BI$31+AJ50*$BJ$31+AU50*$BK$31)/SUM($BG$31:$BK$31)</f>
-        <v>16.3176</v>
+        <v>16.317599999999999</v>
       </c>
       <c r="BG50" s="27">
-        <f ref="BG50:BP50" t="shared" si="26">(D50*$BG$31+O50*$BH$31+Z50*$BI$31+AK50*$BJ$31+AV50*$BK$31)/SUM($BG$31:$BK$31)</f>
+        <f t="shared" ref="BG50:BP50" si="26">(D50*$BG$31+O50*$BH$31+Z50*$BI$31+AK50*$BJ$31+AV50*$BK$31)/SUM($BG$31:$BK$31)</f>
         <v>17.206799999999998</v>
       </c>
       <c r="BH50" s="27">
         <f t="shared" si="26"/>
-        <v>25.107</v>
+        <v>25.106999999999999</v>
       </c>
       <c r="BI50" s="27">
         <f t="shared" si="26"/>
-        <v>16.3296</v>
+        <v>16.329599999999999</v>
       </c>
       <c r="BJ50" s="27">
         <f t="shared" si="26"/>
-        <v>6.7506</v>
+        <v>6.7506000000000004</v>
       </c>
       <c r="BK50" s="27">
         <f t="shared" si="26"/>
@@ -15788,16 +15770,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:70">
       <c r="A51" s="15"/>
       <c r="B51" s="1"/>
       <c r="C51" s="144">
-        <f ref="C51:BE51" t="shared" si="27">C13*C32</f>
+        <f t="shared" ref="C51:BE51" si="27">C13*C32</f>
         <v>29.305</v>
       </c>
       <c r="D51" s="108">
         <f t="shared" si="27"/>
-        <v>17.583</v>
+        <v>17.582999999999998</v>
       </c>
       <c r="E51" s="109">
         <f t="shared" si="27"/>
@@ -15805,7 +15787,7 @@
       </c>
       <c r="F51" s="109">
         <f t="shared" si="27"/>
-        <v>17.583</v>
+        <v>17.582999999999998</v>
       </c>
       <c r="G51" s="109">
         <f t="shared" si="27"/>
@@ -15841,7 +15823,7 @@
       </c>
       <c r="O51" s="108">
         <f t="shared" si="27"/>
-        <v>15.078</v>
+        <v>15.077999999999999</v>
       </c>
       <c r="P51" s="109">
         <f t="shared" si="27"/>
@@ -15849,7 +15831,7 @@
       </c>
       <c r="Q51" s="109">
         <f t="shared" si="27"/>
-        <v>15.078</v>
+        <v>15.077999999999999</v>
       </c>
       <c r="R51" s="111">
         <f t="shared" si="27"/>
@@ -15925,11 +15907,11 @@
       </c>
       <c r="AJ51" s="27">
         <f t="shared" si="27"/>
-        <v>34.975</v>
+        <v>34.975000000000001</v>
       </c>
       <c r="AK51" s="109">
         <f t="shared" si="27"/>
-        <v>20.985</v>
+        <v>20.984999999999999</v>
       </c>
       <c r="AL51" s="109">
         <f t="shared" si="27"/>
@@ -15937,11 +15919,11 @@
       </c>
       <c r="AM51" s="109">
         <f t="shared" si="27"/>
-        <v>20.985</v>
+        <v>20.984999999999999</v>
       </c>
       <c r="AN51" s="109">
         <f t="shared" si="27"/>
-        <v>20.985</v>
+        <v>20.984999999999999</v>
       </c>
       <c r="AO51" s="109">
         <f t="shared" si="27"/>
@@ -15969,7 +15951,7 @@
       </c>
       <c r="AU51" s="27">
         <f t="shared" si="27"/>
-        <v>35.295</v>
+        <v>35.295000000000002</v>
       </c>
       <c r="AV51" s="109">
         <f t="shared" si="27"/>
@@ -16013,15 +15995,15 @@
       </c>
       <c r="BF51" s="27">
         <f>(C51*$BG$32+N51*$BH$32+Y51*$BI$32+AJ51*$BJ$32+AU51*$BK$32)/SUM($BG$32:$BK$32)</f>
-        <v>31.385</v>
+        <v>31.385000000000002</v>
       </c>
       <c r="BG51" s="27">
-        <f ref="BG51:BP51" t="shared" si="28">(D51*$BG$32+O51*$BH$32+Z51*$BI$32+AK51*$BJ$32+AV51*$BK$32)/SUM($BG$32:$BK$32)</f>
+        <f t="shared" ref="BG51:BP51" si="28">(D51*$BG$32+O51*$BH$32+Z51*$BI$32+AK51*$BJ$32+AV51*$BK$32)/SUM($BG$32:$BK$32)</f>
         <v>18.831</v>
       </c>
       <c r="BH51" s="27">
         <f t="shared" si="28"/>
-        <v>5.527</v>
+        <v>5.5270000000000001</v>
       </c>
       <c r="BI51" s="27">
         <f t="shared" si="28"/>
@@ -16059,11 +16041,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:70">
       <c r="A52" s="16"/>
       <c r="B52" s="3"/>
       <c r="C52" s="145">
-        <f ref="C52:BE52" t="shared" si="29">C14*C33</f>
+        <f t="shared" ref="C52:BE52" si="29">C14*C33</f>
         <v>0</v>
       </c>
       <c r="D52" s="116">
@@ -16108,23 +16090,23 @@
       </c>
       <c r="N52" s="145">
         <f t="shared" si="29"/>
-        <v>10.03</v>
+        <v>10.029999999999999</v>
       </c>
       <c r="O52" s="116">
         <f t="shared" si="29"/>
-        <v>10.03</v>
+        <v>10.029999999999999</v>
       </c>
       <c r="P52" s="117">
         <f t="shared" si="29"/>
-        <v>6.018</v>
+        <v>6.0179999999999998</v>
       </c>
       <c r="Q52" s="117">
         <f t="shared" si="29"/>
-        <v>6.018</v>
+        <v>6.0179999999999998</v>
       </c>
       <c r="R52" s="119">
         <f t="shared" si="29"/>
-        <v>6.018</v>
+        <v>6.0179999999999998</v>
       </c>
       <c r="S52" s="117">
         <f t="shared" si="29"/>
@@ -16136,7 +16118,7 @@
       </c>
       <c r="U52" s="116">
         <f t="shared" si="29"/>
-        <v>4.012</v>
+        <v>4.0119999999999996</v>
       </c>
       <c r="V52" s="116">
         <f t="shared" si="29"/>
@@ -16240,11 +16222,11 @@
       </c>
       <c r="AU52" s="75">
         <f t="shared" si="29"/>
-        <v>31.795</v>
+        <v>31.795000000000002</v>
       </c>
       <c r="AV52" s="117">
         <f t="shared" si="29"/>
-        <v>30.995</v>
+        <v>30.995000000000001</v>
       </c>
       <c r="AW52" s="117">
         <f t="shared" si="29"/>
@@ -16256,7 +16238,7 @@
       </c>
       <c r="AY52" s="117">
         <f t="shared" si="29"/>
-        <v>18.597</v>
+        <v>18.597000000000001</v>
       </c>
       <c r="AZ52" s="117">
         <f t="shared" si="29"/>
@@ -16287,7 +16269,7 @@
         <v>20.920555555555556</v>
       </c>
       <c r="BG52" s="72">
-        <f ref="BG52:BP52" t="shared" si="30">(D52*$BG$33+O52*$BH$33+Z52*$BI$33+AK52*$BJ$33+AV52*$BK$33)/SUM($BG$33:$BK$33)</f>
+        <f t="shared" ref="BG52:BP52" si="30">(D52*$BG$33+O52*$BH$33+Z52*$BI$33+AK52*$BJ$33+AV52*$BK$33)/SUM($BG$33:$BK$33)</f>
         <v>21.15111111111111</v>
       </c>
       <c r="BH52" s="72">
@@ -16296,7 +16278,7 @@
       </c>
       <c r="BI52" s="72">
         <f t="shared" si="30"/>
-        <v>4.984166666666667</v>
+        <v>4.9841666666666669</v>
       </c>
       <c r="BJ52" s="72">
         <f t="shared" si="30"/>
@@ -16330,11 +16312,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:70">
       <c r="A53" s="149"/>
       <c r="B53" s="2"/>
       <c r="C53" s="143">
-        <f ref="C53:BE53" t="shared" si="31">C15*C34</f>
+        <f t="shared" ref="C53:BE53" si="31">C15*C34</f>
         <v>0</v>
       </c>
       <c r="D53" s="121">
@@ -16558,7 +16540,7 @@
         <v>0</v>
       </c>
       <c r="BG53" s="26">
-        <f ref="BG53:BP53" t="shared" si="32">(D53*$BG$34+O53*$BH$34+Z53*$BI$34+AK53*$BJ$34+AV53*$BK$34)/SUM($BG$34:$BK$34)</f>
+        <f t="shared" ref="BG53:BP53" si="32">(D53*$BG$34+O53*$BH$34+Z53*$BI$34+AK53*$BJ$34+AV53*$BK$34)/SUM($BG$34:$BK$34)</f>
         <v>0</v>
       </c>
       <c r="BH53" s="26">
@@ -16601,11 +16583,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:70">
       <c r="A54" s="15"/>
       <c r="B54" s="1"/>
       <c r="C54" s="144">
-        <f ref="C54:BE54" t="shared" si="33">C16*C35</f>
+        <f t="shared" ref="C54:BE54" si="33">C16*C35</f>
         <v>0</v>
       </c>
       <c r="D54" s="108">
@@ -16829,7 +16811,7 @@
         <v>0</v>
       </c>
       <c r="BG54" s="27">
-        <f ref="BG54:BP54" t="shared" si="34">(D54*$BG$35+O54*$BH$35+Z54*$BI$35+AK54*$BJ$35+AV54*$BK$35)/SUM($BG$35:$BK$35)</f>
+        <f t="shared" ref="BG54:BP54" si="34">(D54*$BG$35+O54*$BH$35+Z54*$BI$35+AK54*$BJ$35+AV54*$BK$35)/SUM($BG$35:$BK$35)</f>
         <v>32.5</v>
       </c>
       <c r="BH54" s="27">
@@ -16872,11 +16854,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:70">
       <c r="A55" s="129"/>
       <c r="B55" s="3"/>
       <c r="C55" s="145">
-        <f ref="C55:BE55" t="shared" si="35">C17*C36</f>
+        <f t="shared" ref="C55:BE55" si="35">C17*C36</f>
         <v>0</v>
       </c>
       <c r="D55" s="116">
@@ -17100,7 +17082,7 @@
         <v>0</v>
       </c>
       <c r="BG55" s="75">
-        <f ref="BG55:BP55" t="shared" si="36">(D55*$BG$36+O55*$BH$36+Z55*$BI$36+AK55*$BJ$36+AV55*$BK$36)/SUM($BG$35:$BK$35)</f>
+        <f t="shared" ref="BG55:BP55" si="36">(D55*$BG$36+O55*$BH$36+Z55*$BI$36+AK55*$BJ$36+AV55*$BK$36)/SUM($BG$35:$BK$35)</f>
         <v>0</v>
       </c>
       <c r="BH55" s="75">
@@ -17143,7 +17125,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:70">
       <c r="BB57" s="160" t="s">
         <v>60</v>
       </c>
@@ -17156,7 +17138,7 @@
       </c>
       <c r="BG57" s="97">
         <f>(BG41*BR41+BG42*BR42+BG43*BR43+BG49*BR49+BG50*BR50+BG51*BR51+BG52*BR52+BG54*BR54)/(BR41+BR42+BR43+BR49+BR50+BR51+BR52+BR54)</f>
-        <v>21.0855712345679</v>
+        <v>21.085571234567901</v>
       </c>
       <c r="BH57" s="97">
         <f>(BH41*BR41+BH42*BR42+BH43*BR43+BH49*BR49+BH50*BR50+BH51*BR51+BH52*BR52+BH54*BR54)/(BR41+BR42+BR43+BR49+BR50+BR51+BR52+BR54)</f>
@@ -17168,15 +17150,15 @@
       </c>
       <c r="BJ57" s="97">
         <f>(BJ41*BR41+BJ43*BR43+BJ44*BR44+BJ50*BR50+BJ51*BR51+BJ52*BR52+BJ54*BR54)/(BR41+BR43+BR44+BR50+BR51+BR52+BR54)</f>
-        <v>19.02856111111111</v>
+        <v>19.028561111111109</v>
       </c>
       <c r="BK57" s="97">
         <f>(BK41*BR41+BK44*BR44+BK54*BR54)/(BR41+BR44+BR54)</f>
-        <v>23.346515625</v>
+        <v>23.346515624999999</v>
       </c>
       <c r="BL57" s="97">
         <f>(BL46*BR46+BL47*BR47+BL54*BR54)/(BR46+BR47+BR54)</f>
-        <v>21.7856</v>
+        <v>21.785599999999999</v>
       </c>
       <c r="BM57" s="97">
         <f>(BM43*BR43+BM52*BR52+BM54*BR54)/(BR43+BR52+BR54)</f>
@@ -17192,32 +17174,32 @@
       </c>
       <c r="BP57" s="98">
         <f>(BP41*BR41+BP43*BR43)/(BR41+BR43)</f>
-        <v>19.572</v>
+        <v>19.571999999999999</v>
       </c>
     </row>
-    <row r="58">
-      <c r="BM58" s="0" t="s">
+    <row r="58" spans="1:70">
+      <c r="BM58" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="60">
-      <c r="K60" s="0" t="s">
+    <row r="60" spans="1:70">
+      <c r="K60" t="s">
         <v>31</v>
       </c>
-      <c r="BD60" s="0" t="s">
+      <c r="BD60" t="s">
         <v>31</v>
       </c>
-      <c r="BK60" s="0" t="s">
+      <c r="BK60" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="63">
-      <c r="C63" s="0" t="s">
+    <row r="63" spans="1:70">
+      <c r="C63" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="25">
     <mergeCell ref="BB57:BE57"/>
     <mergeCell ref="BG20:BL20"/>
     <mergeCell ref="A39:A40"/>
@@ -17245,87 +17227,87 @@
     <mergeCell ref="AJ1:AT1"/>
   </mergeCells>
   <conditionalFormatting sqref="C22:M36">
-    <cfRule type="cellIs" dxfId="0" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="46" operator="greaterThan">
       <formula>0.09</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22:X36">
-    <cfRule type="cellIs" dxfId="0" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="45" operator="greaterThan">
       <formula>0.09</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y22:AI36">
-    <cfRule type="cellIs" dxfId="0" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="44" operator="greaterThan">
       <formula>0.09</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ22:AT36">
-    <cfRule type="cellIs" dxfId="0" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="43" operator="greaterThan">
       <formula>0.09</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU22:BE36">
-    <cfRule type="cellIs" dxfId="0" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="42" operator="greaterThan">
       <formula>0.09</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C55">
-    <cfRule type="cellIs" dxfId="9" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="40" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R41:S55 U41:U55">
-    <cfRule type="cellIs" dxfId="8" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="39" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD41:AE55 AH41:AI55">
-    <cfRule type="cellIs" dxfId="2" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="38" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ41:AT55">
-    <cfRule type="cellIs" dxfId="1" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="37" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU41:BE55">
-    <cfRule type="cellIs" dxfId="5" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="36" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:M55">
-    <cfRule type="cellIs" dxfId="0" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="35" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N41:X55">
-    <cfRule type="cellIs" dxfId="8" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="34" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF41:BP55">
-    <cfRule type="cellIs" dxfId="3" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="33" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y41:AI55">
-    <cfRule type="cellIs" dxfId="2" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="32" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D48">
-    <cfRule type="cellIs" dxfId="9" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="31" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48">
-    <cfRule type="cellIs" dxfId="9" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="30" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L48">
-    <cfRule type="cellIs" dxfId="9" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="29" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17340,12 +17322,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD3:AE17 AH3:AI17">
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3:AT7 AJ9:AT17 AJ8:AO8 AQ8:AT8">
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17355,7 +17337,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:M17">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17381,7 +17363,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>